<commit_message>
CK/CM info updated. HV and TJ drafts started.
</commit_message>
<xml_diff>
--- a/_xml/Abilities.xlsx
+++ b/_xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="130">
   <si>
     <t>Perkinite:</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Conic</t>
   </si>
   <si>
-    <t>If John is in SOS Mode, John gets extra Attack, Defense, and Speed.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enemies nearby Eric lose extra defense. </t>
   </si>
   <si>
@@ -303,7 +300,112 @@
     <t>tentacle_circle</t>
   </si>
   <si>
-    <t>Enemies nearby Eric lose some Health every two seconds.</t>
+    <t>Charles Yeh (CY)</t>
+  </si>
+  <si>
+    <t>Nate Mastropaolo (NM)</t>
+  </si>
+  <si>
+    <t>Christina Kata (CK)</t>
+  </si>
+  <si>
+    <t>Cia Mathew (CM)</t>
+  </si>
+  <si>
+    <t>Eyelash Batting</t>
+  </si>
+  <si>
+    <t>Graceful Dodge</t>
+  </si>
+  <si>
+    <t>Shoe Throwing</t>
+  </si>
+  <si>
+    <t>Mediation - Excessive Cursing</t>
+  </si>
+  <si>
+    <t>Railgun Striker</t>
+  </si>
+  <si>
+    <t>Fires at least four bullets in the direction of the cursor/target.</t>
+  </si>
+  <si>
+    <t>Teleports to where the cursor is instantly.</t>
+  </si>
+  <si>
+    <t>Sedated Needles</t>
+  </si>
+  <si>
+    <t>Strikes enemies with knitting needles laced with sedatives, slowing them down slightly for 3 seconds.</t>
+  </si>
+  <si>
+    <t>Cheer!</t>
+  </si>
+  <si>
+    <t>Cia and Kata restore extra Health every 5 seconds.</t>
+  </si>
+  <si>
+    <t>Living the Dream</t>
+  </si>
+  <si>
+    <t>Durations of Cia's Buffs are increased by 15%. Durations of Cia's Debuffs are decreased by 30%.</t>
+  </si>
+  <si>
+    <t>love</t>
+  </si>
+  <si>
+    <t>curse</t>
+  </si>
+  <si>
+    <t>health_up</t>
+  </si>
+  <si>
+    <t>Ranged Attacker</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Melee Attacker</t>
+  </si>
+  <si>
+    <t>Hybrid Attacker</t>
+  </si>
+  <si>
+    <t>While John is in SOS Mode, John gets extra Attack, Defense, and Speed.</t>
+  </si>
+  <si>
+    <t>If Kata reaches SOS Mode, Kata stuns all enemies within a large area for three seconds. This ability refreshes every 60 seconds.</t>
+  </si>
+  <si>
+    <t>Enemies nearby Eric are damaged, silenced for 1 second, and are slowed for 2 seconds every 5 seconds.</t>
+  </si>
+  <si>
+    <t>Debuff Support</t>
+  </si>
+  <si>
+    <t>All-Around Support</t>
+  </si>
+  <si>
+    <t>Assassin</t>
+  </si>
+  <si>
+    <t>Kata throws a shoe to the closest enemy every 5 seconds.</t>
+  </si>
+  <si>
+    <t>SOS Setup</t>
+  </si>
+  <si>
+    <t>Sends a love charm in the direction of the cursor, damaging and stunning enemies along the path.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Huong Vong (HV)</t>
+  </si>
+  <si>
+    <t>Huilian Qiu (HQ)</t>
   </si>
 </sst>
 </file>
@@ -469,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -525,35 +627,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -591,6 +674,30 @@
           <color theme="4" tint="0.39997558519241921"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -761,10 +868,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:AY9" tableType="xml" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2">
-  <autoFilter ref="B1:AY9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B1:AY25" tableType="xml" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="B1:AY25"/>
   <tableColumns count="50">
-    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="1">
+    <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="0">
       <xmlColumnPr mapId="3" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="Description" name="Description">
@@ -1207,17 +1314,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AY9"/>
+  <dimension ref="A1:AY34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="116.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="117.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" customWidth="1"/>
@@ -1331,7 +1438,7 @@
         <v>38</v>
       </c>
       <c r="W1" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="X1" s="27" t="s">
         <v>39</v>
@@ -1355,7 +1462,7 @@
         <v>46</v>
       </c>
       <c r="AE1" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AF1" s="27" t="s">
         <v>47</v>
@@ -1420,7 +1527,7 @@
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -1476,7 +1583,7 @@
         <v>50</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X2" s="8">
         <v>15</v>
@@ -1514,6 +1621,9 @@
       <c r="AY2" s="17"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
       <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
@@ -1584,7 +1694,7 @@
         <v>70</v>
       </c>
       <c r="AE3" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF3" s="9">
         <f>32*4</f>
@@ -1594,7 +1704,7 @@
         <v>256</v>
       </c>
       <c r="AH3" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AI3" s="9"/>
       <c r="AJ3" s="9"/>
@@ -1619,11 +1729,14 @@
       <c r="AY3" s="22"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="14">
         <v>5</v>
@@ -1659,7 +1772,7 @@
         <v>48</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
@@ -1701,7 +1814,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D5" s="19">
         <v>9</v>
@@ -1719,7 +1832,7 @@
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="21">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>78</v>
@@ -1737,7 +1850,7 @@
         <v>64</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X5" s="9">
         <v>5</v>
@@ -1765,7 +1878,9 @@
       <c r="AM5" s="9"/>
       <c r="AN5" s="9"/>
       <c r="AO5" s="9"/>
-      <c r="AP5" s="9"/>
+      <c r="AP5" s="32">
+        <v>-15</v>
+      </c>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
@@ -1773,12 +1888,14 @@
       <c r="AU5" s="9"/>
       <c r="AV5" s="9"/>
       <c r="AW5" s="9"/>
-      <c r="AX5" s="9"/>
+      <c r="AX5" s="33">
+        <v>24</v>
+      </c>
       <c r="AY5" s="22"/>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
@@ -1840,7 +1957,7 @@
       <c r="AC6" s="8"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AF6" s="8">
         <v>250</v>
@@ -1849,7 +1966,7 @@
         <v>250</v>
       </c>
       <c r="AH6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8"/>
@@ -1870,6 +1987,9 @@
       <c r="AY6" s="17"/>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
       <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
@@ -1885,7 +2005,9 @@
       <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="H7" s="9" t="s">
         <v>72</v>
       </c>
@@ -1894,7 +2016,7 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L7" s="9">
         <v>300</v>
@@ -1962,6 +2084,9 @@
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -2002,7 +2127,7 @@
         <v>48</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
@@ -2044,7 +2169,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="D9" s="3">
         <v>11</v>
@@ -2111,6 +2236,329 @@
       <c r="AW9" s="4"/>
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B11" s="31"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B12" s="31"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B13" s="31"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B15" s="31"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B16" s="31"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B17" s="31"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <f>28*3</f>
+        <v>84</v>
+      </c>
+      <c r="N18" t="s">
+        <v>76</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>6</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>144</v>
+      </c>
+      <c r="N19" t="s">
+        <v>76</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>76</v>
+      </c>
+      <c r="AS19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="3">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="M20">
+        <v>120</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS20" s="3"/>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B21" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="3">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="M21">
+        <v>1440</v>
+      </c>
+      <c r="N21" t="s">
+        <v>78</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="3">
+        <f>24*3</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>16</v>
+      </c>
+      <c r="N22" t="s">
+        <v>52</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>168</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="3">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="M24">
+        <f>24*5</f>
+        <v>120</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="AM24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="3">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stat and map edits
</commit_message>
<xml_diff>
--- a/_xml/Abilities.xlsx
+++ b/_xml/Abilities.xlsx
@@ -381,9 +381,6 @@
     <t>Mom Swap</t>
   </si>
   <si>
-    <t>Basic Attack: Weaken an enemy with lust.</t>
-  </si>
-  <si>
     <t>Place a booby-trapped fake beard on an enemy, which explodes for massive damage.</t>
   </si>
   <si>
@@ -760,6 +757,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Weaken an enemy with lust.</t>
   </si>
 </sst>
 </file>
@@ -2564,9 +2564,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D41" sqref="D41"/>
+      <selection pane="topRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2608,13 +2608,13 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1">
@@ -2640,79 +2640,79 @@
         <v>3</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="T2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="W2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="W2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="X2" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="Y2" s="7" t="s">
+      <c r="AC2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF2" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:32" s="36" customFormat="1" ht="15.75" thickTop="1">
@@ -2723,7 +2723,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>90</v>
@@ -2735,13 +2735,13 @@
         <v>200</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" s="42">
         <v>400</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J3" s="33"/>
       <c r="K3" s="33"/>
@@ -2787,7 +2787,7 @@
         <v>250</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="33"/>
@@ -2907,7 +2907,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>47</v>
@@ -2919,11 +2919,11 @@
         <v>50</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
@@ -2954,10 +2954,10 @@
         <v>46</v>
       </c>
       <c r="B8" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>211</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>212</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="39">
@@ -2967,11 +2967,11 @@
         <v>270</v>
       </c>
       <c r="G8" s="41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H8" s="34"/>
       <c r="I8" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J8" s="33"/>
       <c r="K8" s="33"/>
@@ -3006,7 +3006,7 @@
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" s="14">
         <v>0</v>
@@ -3027,7 +3027,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
       <c r="U9" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
@@ -3044,7 +3044,7 @@
         <v>89</v>
       </c>
       <c r="AF9" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="19" customFormat="1">
@@ -3078,7 +3078,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
       <c r="V10" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="W10" s="15"/>
       <c r="X10" s="17"/>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="14">
         <v>1</v>
@@ -3138,11 +3138,11 @@
         <v>46</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" s="14">
         <v>3</v>
@@ -3195,11 +3195,11 @@
         <v>340</v>
       </c>
       <c r="G13" s="33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H13" s="34"/>
       <c r="I13" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
@@ -3233,10 +3233,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E14" s="32">
         <v>1</v>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="H14" s="34"/>
       <c r="I14" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J14" s="33"/>
       <c r="K14" s="33"/>
@@ -3326,7 +3326,7 @@
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16" s="14">
         <v>3</v>
@@ -3367,10 +3367,10 @@
         <v>86</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E17" s="32">
         <v>8</v>
@@ -3379,11 +3379,11 @@
         <v>200</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="33" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
@@ -3420,7 +3420,7 @@
         <v>87</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E18" s="32">
         <v>1</v>
@@ -3429,11 +3429,11 @@
         <v>200</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H18" s="34"/>
       <c r="I18" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20" s="14">
         <v>2</v>
@@ -3548,11 +3548,11 @@
         <v>8</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" s="14">
         <v>0</v>
@@ -3573,7 +3573,7 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
       <c r="U21" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
@@ -3583,14 +3583,14 @@
       <c r="AA21" s="15"/>
       <c r="AB21" s="15"/>
       <c r="AC21" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AD21" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AE21" s="15"/>
       <c r="AF21" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:32" s="36" customFormat="1">
@@ -3598,10 +3598,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>104</v>
@@ -3613,11 +3613,11 @@
         <v>400</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H22" s="34"/>
       <c r="I22" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
@@ -3648,10 +3648,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>76</v>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H23" s="34"/>
       <c r="I23" s="33"/>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E24" s="14">
         <v>1</v>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E25" s="14">
         <v>1</v>
@@ -3820,10 +3820,10 @@
         <v>49</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>50</v>
@@ -3835,11 +3835,11 @@
         <v>50</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H27" s="34"/>
       <c r="I27" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
@@ -3870,7 +3870,7 @@
         <v>49</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>87</v>
@@ -3885,7 +3885,7 @@
         <v>100</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H28" s="34"/>
       <c r="I28" s="33"/>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E30" s="14">
         <v>1</v>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E31" s="14">
         <v>0</v>
@@ -4017,7 +4017,7 @@
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
@@ -4029,7 +4029,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
       <c r="U31" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="V31" s="15"/>
       <c r="W31" s="15"/>
@@ -4040,11 +4040,11 @@
       <c r="AB31" s="15"/>
       <c r="AC31" s="15"/>
       <c r="AD31" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AE31" s="15"/>
       <c r="AF31" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:32" s="36" customFormat="1">
@@ -4052,13 +4052,13 @@
         <v>55</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E32" s="32">
         <v>1</v>
@@ -4102,13 +4102,13 @@
         <v>55</v>
       </c>
       <c r="B33" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D33" s="44" t="s">
         <v>240</v>
-      </c>
-      <c r="C33" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>241</v>
       </c>
       <c r="E33" s="32">
         <v>1</v>
@@ -4117,11 +4117,11 @@
         <v>70</v>
       </c>
       <c r="G33" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H33" s="34"/>
       <c r="I33" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J33" s="33"/>
       <c r="K33" s="33"/>
@@ -4245,16 +4245,16 @@
     </row>
     <row r="36" spans="1:32" s="36" customFormat="1">
       <c r="A36" s="37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B36" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36" s="44" t="s">
         <v>242</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>243</v>
       </c>
       <c r="E36" s="38">
         <v>1</v>
@@ -4263,11 +4263,11 @@
         <v>80</v>
       </c>
       <c r="G36" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H36" s="34"/>
       <c r="I36" s="46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J36" s="33"/>
       <c r="K36" s="33"/>
@@ -4295,16 +4295,16 @@
     </row>
     <row r="37" spans="1:32" s="36" customFormat="1">
       <c r="A37" s="37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="D37" s="44" t="s">
         <v>244</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="D37" s="44" t="s">
-        <v>245</v>
       </c>
       <c r="E37" s="39">
         <v>1</v>
@@ -4313,7 +4313,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H37" s="34"/>
       <c r="I37" s="41">
@@ -4345,14 +4345,14 @@
     </row>
     <row r="38" spans="1:32" s="19" customFormat="1">
       <c r="A38" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>132</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>133</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E38" s="20">
         <v>1</v>
@@ -4393,14 +4393,14 @@
     </row>
     <row r="39" spans="1:32" s="19" customFormat="1">
       <c r="A39" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" s="20">
         <v>0</v>
@@ -4447,7 +4447,7 @@
         <v>64</v>
       </c>
       <c r="C40" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D40" s="31" t="s">
         <v>69</v>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="H40" s="34"/>
       <c r="I40" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J40" s="33"/>
       <c r="K40" s="33"/>
@@ -4497,7 +4497,7 @@
         <v>65</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>95</v>
@@ -4643,10 +4643,10 @@
         <v>119</v>
       </c>
       <c r="C44" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="D44" s="31" t="s">
-        <v>121</v>
+        <v>212</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>247</v>
       </c>
       <c r="E44" s="32">
         <v>1</v>
@@ -4655,11 +4655,11 @@
         <v>250</v>
       </c>
       <c r="G44" s="46" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J44" s="33"/>
       <c r="K44" s="33"/>
@@ -4693,10 +4693,10 @@
         <v>118</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E45" s="39">
         <v>1</v>
@@ -4705,11 +4705,11 @@
         <v>200</v>
       </c>
       <c r="G45" s="47" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H45" s="34"/>
       <c r="I45" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J45" s="33"/>
       <c r="K45" s="33"/>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E46" s="20">
         <v>1</v>
@@ -4792,7 +4792,7 @@
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" s="20">
         <v>1</v>
@@ -4840,7 +4840,7 @@
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E48" s="20">
         <v>1</v>
@@ -5032,7 +5032,7 @@
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E52" s="14">
         <v>5</v>
@@ -5464,7 +5464,7 @@
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E61" s="14">
         <v>3</v>
@@ -5512,7 +5512,7 @@
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E62" s="14">
         <v>1</v>
@@ -5560,7 +5560,7 @@
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E63" s="14">
         <v>1</v>
@@ -5604,11 +5604,11 @@
         <v>70</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E64" s="14">
         <v>1</v>
@@ -5649,14 +5649,14 @@
     </row>
     <row r="65" spans="1:32" s="19" customFormat="1">
       <c r="A65" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E65" s="14"/>
       <c r="F65" s="14"/>
@@ -5689,14 +5689,14 @@
     </row>
     <row r="66" spans="1:32" s="19" customFormat="1">
       <c r="A66" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>173</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
@@ -5729,14 +5729,14 @@
     </row>
     <row r="67" spans="1:32" s="19" customFormat="1">
       <c r="A67" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
@@ -5769,14 +5769,14 @@
     </row>
     <row r="68" spans="1:32" s="19" customFormat="1">
       <c r="A68" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
@@ -5860,11 +5860,11 @@
         <v>36</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E70" s="20">
         <v>1</v>
@@ -6244,11 +6244,11 @@
         <v>36</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="21"/>
@@ -6284,11 +6284,11 @@
         <v>36</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="21"/>
@@ -6324,11 +6324,11 @@
         <v>36</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="21"/>
@@ -6364,11 +6364,11 @@
         <v>36</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="21"/>
@@ -6404,11 +6404,11 @@
         <v>36</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="21"/>
@@ -6444,11 +6444,11 @@
         <v>36</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E83" s="20">
         <v>0</v>
@@ -6492,11 +6492,11 @@
         <v>36</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E84" s="20">
         <v>0</v>
@@ -6540,11 +6540,11 @@
         <v>36</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E85" s="20">
         <v>0</v>
@@ -6586,11 +6586,11 @@
     <row r="86" spans="1:33" s="19" customFormat="1">
       <c r="A86" s="23"/>
       <c r="B86" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C86" s="23"/>
       <c r="D86" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E86" s="25"/>
       <c r="F86" s="25"/>

</xml_diff>

<commit_message>
map database working, face icons being loaded
</commit_message>
<xml_diff>
--- a/_xml/Abilities.xlsx
+++ b/_xml/Abilities.xlsx
@@ -168,9 +168,6 @@
     <t>Cia M.</t>
   </si>
   <si>
-    <t>Basic Attack: Shoot beams of magic to targets.</t>
-  </si>
-  <si>
     <t>V.P.S.</t>
   </si>
   <si>
@@ -790,6 +787,9 @@
   </si>
   <si>
     <t>Modify Movement Speed with new clothes, and also dazzle nearby enemies.</t>
+  </si>
+  <si>
+    <t>Throws needles that slow the enemy</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -980,13 +980,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1080,16 +1095,28 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="2" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -2621,9 +2648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B40" sqref="B40:AF40"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A40" sqref="A40:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2631,7 +2658,7 @@
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
@@ -2665,13 +2692,13 @@
   <sheetData>
     <row r="1" spans="1:32">
       <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>129</v>
-      </c>
-      <c r="E1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="15.75" thickBot="1">
@@ -2697,79 +2724,79 @@
         <v>3</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="T2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="V2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="S2" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="W2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="W2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="X2" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="Y2" s="7" t="s">
+      <c r="AC2" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF2" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD2" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:32" s="35" customFormat="1" ht="15.75" thickTop="1">
@@ -2780,10 +2807,10 @@
         <v>26</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="37">
         <v>1</v>
@@ -2792,13 +2819,13 @@
         <v>200</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H3" s="41">
         <v>400</v>
       </c>
       <c r="I3" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
@@ -2832,10 +2859,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="31">
         <v>1</v>
@@ -2844,7 +2871,7 @@
         <v>250</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H4" s="41"/>
       <c r="I4" s="32"/>
@@ -2881,7 +2908,7 @@
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" s="13">
         <v>1</v>
@@ -2923,7 +2950,7 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" s="14">
         <v>1</v>
@@ -2964,7 +2991,7 @@
         <v>42</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>47</v>
@@ -2976,11 +3003,11 @@
         <v>50</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
@@ -3011,10 +3038,10 @@
         <v>46</v>
       </c>
       <c r="B8" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>210</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>211</v>
       </c>
       <c r="D8" s="30"/>
       <c r="E8" s="38">
@@ -3024,11 +3051,11 @@
         <v>270</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H8" s="33"/>
       <c r="I8" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
@@ -3063,7 +3090,7 @@
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E9" s="14">
         <v>0</v>
@@ -3084,7 +3111,7 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
       <c r="U9" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V9" s="15"/>
       <c r="W9" s="15"/>
@@ -3098,10 +3125,10 @@
       </c>
       <c r="AD9" s="15"/>
       <c r="AE9" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF9" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:32" s="19" customFormat="1">
@@ -3113,7 +3140,7 @@
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="14">
         <v>1</v>
@@ -3135,7 +3162,7 @@
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
       <c r="V10" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="W10" s="15"/>
       <c r="X10" s="17"/>
@@ -3157,7 +3184,7 @@
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E11" s="14">
         <v>1</v>
@@ -3195,11 +3222,11 @@
         <v>46</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E12" s="14">
         <v>3</v>
@@ -3240,10 +3267,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="31">
         <v>1</v>
@@ -3252,11 +3279,11 @@
         <v>340</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
@@ -3290,10 +3317,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E14" s="31">
         <v>1</v>
@@ -3306,7 +3333,7 @@
       </c>
       <c r="H14" s="33"/>
       <c r="I14" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
@@ -3379,11 +3406,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E16" s="14">
         <v>3</v>
@@ -3421,13 +3448,13 @@
         <v>8</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E17" s="31">
         <v>8</v>
@@ -3436,11 +3463,11 @@
         <v>200</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H17" s="33"/>
       <c r="I17" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
@@ -3474,10 +3501,10 @@
         <v>9</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E18" s="31">
         <v>1</v>
@@ -3486,11 +3513,11 @@
         <v>200</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
@@ -3567,7 +3594,7 @@
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E20" s="14">
         <v>2</v>
@@ -3605,11 +3632,11 @@
         <v>8</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E21" s="14">
         <v>0</v>
@@ -3630,7 +3657,7 @@
       <c r="S21" s="15"/>
       <c r="T21" s="15"/>
       <c r="U21" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V21" s="15"/>
       <c r="W21" s="15"/>
@@ -3640,14 +3667,14 @@
       <c r="AA21" s="15"/>
       <c r="AB21" s="15"/>
       <c r="AC21" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AD21" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AE21" s="15"/>
       <c r="AF21" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:32" s="35" customFormat="1">
@@ -3655,13 +3682,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E22" s="31">
         <v>1</v>
@@ -3670,11 +3697,11 @@
         <v>400</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H22" s="33"/>
       <c r="I22" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
@@ -3705,20 +3732,20 @@
         <v>7</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="31">
         <v>1</v>
       </c>
       <c r="F23" s="31"/>
       <c r="G23" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H23" s="33"/>
       <c r="I23" s="32"/>
@@ -3755,7 +3782,7 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E24" s="14">
         <v>1</v>
@@ -3793,11 +3820,11 @@
         <v>7</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E25" s="14">
         <v>1</v>
@@ -3835,11 +3862,11 @@
         <v>7</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" s="14">
         <v>1</v>
@@ -3877,13 +3904,13 @@
         <v>49</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>50</v>
+        <v>211</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>257</v>
       </c>
       <c r="E27" s="31">
         <v>1</v>
@@ -3892,11 +3919,11 @@
         <v>50</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H27" s="33"/>
       <c r="I27" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
@@ -3927,13 +3954,13 @@
         <v>49</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" s="31">
         <v>1</v>
@@ -3942,7 +3969,7 @@
         <v>100</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H28" s="33"/>
       <c r="I28" s="32"/>
@@ -3975,11 +4002,11 @@
         <v>49</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" s="14">
         <v>1</v>
@@ -4017,11 +4044,11 @@
         <v>49</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E30" s="14">
         <v>1</v>
@@ -4059,11 +4086,11 @@
         <v>49</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E31" s="14">
         <v>0</v>
@@ -4074,7 +4101,7 @@
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
       <c r="K31" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
@@ -4086,7 +4113,7 @@
       <c r="S31" s="15"/>
       <c r="T31" s="15"/>
       <c r="U31" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V31" s="15"/>
       <c r="W31" s="15"/>
@@ -4097,25 +4124,25 @@
       <c r="AB31" s="15"/>
       <c r="AC31" s="15"/>
       <c r="AD31" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AE31" s="15"/>
       <c r="AF31" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:32" s="35" customFormat="1">
       <c r="A32" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D32" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E32" s="31">
         <v>1</v>
@@ -4156,16 +4183,16 @@
     </row>
     <row r="33" spans="1:33" s="35" customFormat="1">
       <c r="A33" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="43" t="s">
         <v>239</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>212</v>
-      </c>
-      <c r="D33" s="43" t="s">
-        <v>240</v>
       </c>
       <c r="E33" s="31">
         <v>1</v>
@@ -4174,11 +4201,11 @@
         <v>70</v>
       </c>
       <c r="G33" s="45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J33" s="32"/>
       <c r="K33" s="32"/>
@@ -4206,14 +4233,14 @@
     </row>
     <row r="34" spans="1:33" s="19" customFormat="1">
       <c r="A34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E34" s="14">
         <v>1</v>
@@ -4254,14 +4281,14 @@
     </row>
     <row r="35" spans="1:33" s="19" customFormat="1">
       <c r="A35" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E35" s="14">
         <v>1</v>
@@ -4302,16 +4329,16 @@
     </row>
     <row r="36" spans="1:33" s="35" customFormat="1">
       <c r="A36" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" s="44" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" s="43" t="s">
         <v>241</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>212</v>
-      </c>
-      <c r="D36" s="43" t="s">
-        <v>242</v>
       </c>
       <c r="E36" s="37">
         <v>1</v>
@@ -4320,11 +4347,11 @@
         <v>80</v>
       </c>
       <c r="G36" s="45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H36" s="33"/>
       <c r="I36" s="45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J36" s="32"/>
       <c r="K36" s="32"/>
@@ -4352,16 +4379,16 @@
     </row>
     <row r="37" spans="1:33" s="35" customFormat="1">
       <c r="A37" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37" s="42" t="s">
+        <v>242</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="D37" s="43" t="s">
         <v>243</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>213</v>
-      </c>
-      <c r="D37" s="43" t="s">
-        <v>244</v>
       </c>
       <c r="E37" s="38">
         <v>1</v>
@@ -4370,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="40">
@@ -4402,14 +4429,14 @@
     </row>
     <row r="38" spans="1:33" s="19" customFormat="1">
       <c r="A38" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E38" s="20">
         <v>1</v>
@@ -4450,14 +4477,14 @@
     </row>
     <row r="39" spans="1:33" s="19" customFormat="1">
       <c r="A39" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E39" s="20">
         <v>0</v>
@@ -4496,179 +4523,179 @@
       <c r="AE39" s="15"/>
       <c r="AF39" s="17"/>
     </row>
-    <row r="40" spans="1:33" s="19" customFormat="1">
-      <c r="A40" s="47" t="s">
+    <row r="40" spans="1:33" s="35" customFormat="1">
+      <c r="A40" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="E40" s="49"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="53"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="53"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53"/>
+      <c r="T40" s="53"/>
+      <c r="U40" s="53"/>
+      <c r="V40" s="53"/>
+      <c r="W40" s="53"/>
+      <c r="X40" s="53"/>
+      <c r="Y40" s="53"/>
+      <c r="Z40" s="53"/>
+      <c r="AA40" s="53"/>
+      <c r="AB40" s="53"/>
+      <c r="AC40" s="53"/>
+      <c r="AD40" s="53"/>
+      <c r="AE40" s="53"/>
+      <c r="AF40" s="54"/>
+      <c r="AG40" s="53"/>
+    </row>
+    <row r="41" spans="1:33" s="35" customFormat="1">
+      <c r="A41" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48" t="s">
+        <v>253</v>
+      </c>
+      <c r="E41" s="49"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="52"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="53"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="53"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53"/>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="53"/>
+      <c r="Y41" s="53"/>
+      <c r="Z41" s="53"/>
+      <c r="AA41" s="53"/>
+      <c r="AB41" s="53"/>
+      <c r="AC41" s="53"/>
+      <c r="AD41" s="53"/>
+      <c r="AE41" s="53"/>
+      <c r="AF41" s="54"/>
+    </row>
+    <row r="42" spans="1:33" s="35" customFormat="1">
+      <c r="A42" s="56" t="s">
         <v>248</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24" t="s">
+      <c r="B42" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="C42" s="47"/>
+      <c r="D42" s="48" t="s">
+        <v>256</v>
+      </c>
+      <c r="E42" s="49"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="53"/>
+      <c r="Y42" s="53"/>
+      <c r="Z42" s="53"/>
+      <c r="AA42" s="53"/>
+      <c r="AB42" s="53"/>
+      <c r="AC42" s="53"/>
+      <c r="AD42" s="53"/>
+      <c r="AE42" s="53"/>
+      <c r="AF42" s="54"/>
+    </row>
+    <row r="43" spans="1:33" s="35" customFormat="1">
+      <c r="A43" s="56" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="48" t="s">
         <v>255</v>
       </c>
-      <c r="E40" s="48"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="R40" s="27"/>
-      <c r="S40" s="27"/>
-      <c r="T40" s="27"/>
-      <c r="U40" s="27"/>
-      <c r="V40" s="27"/>
-      <c r="W40" s="27"/>
-      <c r="X40" s="27"/>
-      <c r="Y40" s="27"/>
-      <c r="Z40" s="27"/>
-      <c r="AA40" s="27"/>
-      <c r="AB40" s="27"/>
-      <c r="AC40" s="27"/>
-      <c r="AD40" s="27"/>
-      <c r="AE40" s="27"/>
-      <c r="AF40" s="28"/>
-      <c r="AG40" s="27"/>
-    </row>
-    <row r="41" spans="1:33">
-      <c r="A41" s="47" t="s">
-        <v>248</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="E41" s="48"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
-      <c r="T41" s="27"/>
-      <c r="U41" s="27"/>
-      <c r="V41" s="27"/>
-      <c r="W41" s="27"/>
-      <c r="X41" s="27"/>
-      <c r="Y41" s="27"/>
-      <c r="Z41" s="27"/>
-      <c r="AA41" s="27"/>
-      <c r="AB41" s="27"/>
-      <c r="AC41" s="27"/>
-      <c r="AD41" s="27"/>
-      <c r="AE41" s="27"/>
-      <c r="AF41" s="28"/>
-    </row>
-    <row r="42" spans="1:33">
-      <c r="A42" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>252</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="E42" s="48"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="27"/>
-      <c r="T42" s="27"/>
-      <c r="U42" s="27"/>
-      <c r="V42" s="27"/>
-      <c r="W42" s="27"/>
-      <c r="X42" s="27"/>
-      <c r="Y42" s="27"/>
-      <c r="Z42" s="27"/>
-      <c r="AA42" s="27"/>
-      <c r="AB42" s="27"/>
-      <c r="AC42" s="27"/>
-      <c r="AD42" s="27"/>
-      <c r="AE42" s="27"/>
-      <c r="AF42" s="28"/>
-    </row>
-    <row r="43" spans="1:33">
-      <c r="A43" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>253</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="E43" s="48"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27"/>
-      <c r="T43" s="27"/>
-      <c r="U43" s="27"/>
-      <c r="V43" s="27"/>
-      <c r="W43" s="27"/>
-      <c r="X43" s="27"/>
-      <c r="Y43" s="27"/>
-      <c r="Z43" s="27"/>
-      <c r="AA43" s="27"/>
-      <c r="AB43" s="27"/>
-      <c r="AC43" s="27"/>
-      <c r="AD43" s="27"/>
-      <c r="AE43" s="27"/>
-      <c r="AF43" s="28"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53"/>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
+      <c r="Y43" s="53"/>
+      <c r="Z43" s="53"/>
+      <c r="AA43" s="53"/>
+      <c r="AB43" s="53"/>
+      <c r="AC43" s="53"/>
+      <c r="AD43" s="53"/>
+      <c r="AE43" s="53"/>
+      <c r="AF43" s="54"/>
     </row>
     <row r="44" spans="1:33" s="35" customFormat="1">
       <c r="A44" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="29" t="s">
-        <v>64</v>
-      </c>
       <c r="C44" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="31">
         <v>1</v>
@@ -4681,7 +4708,7 @@
       </c>
       <c r="H44" s="33"/>
       <c r="I44" s="45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J44" s="32"/>
       <c r="K44" s="32"/>
@@ -4709,16 +4736,16 @@
     </row>
     <row r="45" spans="1:33" s="35" customFormat="1">
       <c r="A45" s="42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E45" s="31">
         <v>1</v>
@@ -4759,14 +4786,14 @@
     </row>
     <row r="46" spans="1:33" s="19" customFormat="1">
       <c r="A46" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" s="14">
         <v>3</v>
@@ -4807,14 +4834,14 @@
     </row>
     <row r="47" spans="1:33" s="19" customFormat="1">
       <c r="A47" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E47" s="14">
         <v>1</v>
@@ -4855,16 +4882,16 @@
     </row>
     <row r="48" spans="1:33" s="35" customFormat="1">
       <c r="A48" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D48" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E48" s="31">
         <v>1</v>
@@ -4873,11 +4900,11 @@
         <v>250</v>
       </c>
       <c r="G48" s="45" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H48" s="33"/>
       <c r="I48" s="45" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J48" s="32"/>
       <c r="K48" s="32"/>
@@ -4905,16 +4932,16 @@
     </row>
     <row r="49" spans="1:32" s="35" customFormat="1">
       <c r="A49" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E49" s="38">
         <v>1</v>
@@ -4923,11 +4950,11 @@
         <v>200</v>
       </c>
       <c r="G49" s="46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H49" s="33"/>
       <c r="I49" s="45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J49" s="32"/>
       <c r="K49" s="32"/>
@@ -4955,14 +4982,14 @@
     </row>
     <row r="50" spans="1:32" s="19" customFormat="1">
       <c r="A50" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E50" s="20">
         <v>1</v>
@@ -5003,14 +5030,14 @@
     </row>
     <row r="51" spans="1:32" s="19" customFormat="1">
       <c r="A51" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E51" s="20">
         <v>1</v>
@@ -5051,14 +5078,14 @@
     </row>
     <row r="52" spans="1:32" s="19" customFormat="1">
       <c r="A52" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E52" s="20">
         <v>1</v>
@@ -5250,7 +5277,7 @@
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E56" s="14">
         <v>5</v>
@@ -5291,14 +5318,14 @@
     </row>
     <row r="57" spans="1:32" s="19" customFormat="1">
       <c r="A57" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C57" s="11"/>
       <c r="D57" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E57" s="20">
         <v>1</v>
@@ -5339,14 +5366,14 @@
     </row>
     <row r="58" spans="1:32" s="19" customFormat="1">
       <c r="A58" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E58" s="14">
         <v>1</v>
@@ -5387,14 +5414,14 @@
     </row>
     <row r="59" spans="1:32" s="19" customFormat="1">
       <c r="A59" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E59" s="20">
         <v>1</v>
@@ -5435,14 +5462,14 @@
     </row>
     <row r="60" spans="1:32" s="19" customFormat="1">
       <c r="A60" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E60" s="20">
         <v>1</v>
@@ -5483,14 +5510,14 @@
     </row>
     <row r="61" spans="1:32" s="19" customFormat="1">
       <c r="A61" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>83</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E61" s="14">
         <v>0</v>
@@ -5531,14 +5558,14 @@
     </row>
     <row r="62" spans="1:32" s="19" customFormat="1">
       <c r="A62" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E62" s="14">
         <v>1</v>
@@ -5579,14 +5606,14 @@
     </row>
     <row r="63" spans="1:32" s="19" customFormat="1">
       <c r="A63" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E63" s="14">
         <v>10</v>
@@ -5627,14 +5654,14 @@
     </row>
     <row r="64" spans="1:32" s="19" customFormat="1">
       <c r="A64" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E64" s="14">
         <v>10</v>
@@ -5675,14 +5702,14 @@
     </row>
     <row r="65" spans="1:32" s="19" customFormat="1">
       <c r="A65" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>71</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E65" s="14">
         <v>3</v>
@@ -5723,14 +5750,14 @@
     </row>
     <row r="66" spans="1:32" s="19" customFormat="1">
       <c r="A66" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E66" s="14">
         <v>1</v>
@@ -5771,14 +5798,14 @@
     </row>
     <row r="67" spans="1:32" s="19" customFormat="1">
       <c r="A67" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E67" s="14">
         <v>1</v>
@@ -5819,14 +5846,14 @@
     </row>
     <row r="68" spans="1:32" s="19" customFormat="1">
       <c r="A68" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E68" s="14">
         <v>1</v>
@@ -5867,14 +5894,14 @@
     </row>
     <row r="69" spans="1:32" s="19" customFormat="1">
       <c r="A69" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
@@ -5907,14 +5934,14 @@
     </row>
     <row r="70" spans="1:32" s="19" customFormat="1">
       <c r="A70" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
@@ -5947,14 +5974,14 @@
     </row>
     <row r="71" spans="1:32" s="19" customFormat="1">
       <c r="A71" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
@@ -5987,14 +6014,14 @@
     </row>
     <row r="72" spans="1:32" s="19" customFormat="1">
       <c r="A72" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
@@ -6034,7 +6061,7 @@
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E73" s="14">
         <v>1</v>
@@ -6078,11 +6105,11 @@
         <v>36</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E74" s="20">
         <v>1</v>
@@ -6130,7 +6157,7 @@
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E75" s="14">
         <v>0</v>
@@ -6178,7 +6205,7 @@
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E76" s="14">
         <v>0</v>
@@ -6226,7 +6253,7 @@
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E77" s="14">
         <v>0</v>
@@ -6274,7 +6301,7 @@
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E78" s="14">
         <v>0</v>
@@ -6414,11 +6441,11 @@
         <v>31</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E81" s="20">
         <v>0</v>
@@ -6462,11 +6489,11 @@
         <v>36</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="21"/>
@@ -6502,11 +6529,11 @@
         <v>36</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="21"/>
@@ -6542,11 +6569,11 @@
         <v>36</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="21"/>
@@ -6582,11 +6609,11 @@
         <v>36</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="21"/>
@@ -6622,11 +6649,11 @@
         <v>36</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="21"/>
@@ -6662,11 +6689,11 @@
         <v>36</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E87" s="20">
         <v>0</v>
@@ -6710,11 +6737,11 @@
         <v>36</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E88" s="20">
         <v>0</v>
@@ -6758,11 +6785,11 @@
         <v>36</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E89" s="20">
         <v>0</v>
@@ -6804,11 +6831,11 @@
     <row r="90" spans="1:32" s="19" customFormat="1">
       <c r="A90" s="23"/>
       <c r="B90" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C90" s="23"/>
       <c r="D90" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E90" s="25"/>
       <c r="F90" s="25"/>

</xml_diff>

<commit_message>
xml and teleport points added
</commit_message>
<xml_diff>
--- a/_xml/Abilities.xlsx
+++ b/_xml/Abilities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="298">
   <si>
     <t>Name</t>
   </si>
@@ -874,6 +874,42 @@
   </si>
   <si>
     <t>Richard B.</t>
+  </si>
+  <si>
+    <t>Viet T.</t>
+  </si>
+  <si>
+    <t>Mind Reader</t>
+  </si>
+  <si>
+    <t>Binding Chains</t>
+  </si>
+  <si>
+    <t>Trap enemies with chains.</t>
+  </si>
+  <si>
+    <t>Read an enemy's mind.</t>
+  </si>
+  <si>
+    <t>Cone</t>
+  </si>
+  <si>
+    <t>Mauricio P.</t>
+  </si>
+  <si>
+    <t>Shahid M.</t>
+  </si>
+  <si>
+    <t>Instant Naptime</t>
+  </si>
+  <si>
+    <t>Shaving Cream Shield</t>
+  </si>
+  <si>
+    <t>Makes enemies go to sleep instantly.</t>
+  </si>
+  <si>
+    <t>Shield self and partner with a giant Gillette shield.</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1134,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1227,8 +1263,10 @@
     <xf numFmtId="1" fontId="3" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -2375,7 +2413,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B2:AF100" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" dataCellStyle="20% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B2:AF98" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" dataCellStyle="20% - Accent1">
   <tableColumns count="31">
     <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="30" dataCellStyle="20% - Accent1">
       <xmlColumnPr mapId="45" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
@@ -2758,11 +2796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG104"/>
+  <dimension ref="A1:AG110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C65" sqref="C65"/>
+      <selection pane="topRight" activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2770,7 +2808,7 @@
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="66.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="85.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
@@ -5014,7 +5052,9 @@
         <v>272</v>
       </c>
       <c r="E48" s="49"/>
-      <c r="F48" s="50"/>
+      <c r="F48" s="50">
+        <v>150</v>
+      </c>
       <c r="G48" s="51"/>
       <c r="H48" s="52"/>
       <c r="I48" s="53"/>
@@ -5056,7 +5096,9 @@
         <v>273</v>
       </c>
       <c r="E49" s="49"/>
-      <c r="F49" s="50"/>
+      <c r="F49" s="50">
+        <v>120</v>
+      </c>
       <c r="G49" s="51"/>
       <c r="H49" s="52"/>
       <c r="I49" s="53"/>
@@ -5098,7 +5140,9 @@
         <v>274</v>
       </c>
       <c r="E50" s="49"/>
-      <c r="F50" s="50"/>
+      <c r="F50" s="50">
+        <v>100</v>
+      </c>
       <c r="G50" s="51"/>
       <c r="H50" s="52"/>
       <c r="I50" s="53"/>
@@ -5140,7 +5184,9 @@
         <v>271</v>
       </c>
       <c r="E51" s="49"/>
-      <c r="F51" s="50"/>
+      <c r="F51" s="50">
+        <v>200</v>
+      </c>
       <c r="G51" s="51"/>
       <c r="H51" s="52"/>
       <c r="I51" s="53"/>
@@ -5851,7 +5897,9 @@
       <c r="B66" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="29"/>
+      <c r="C66" s="42" t="s">
+        <v>86</v>
+      </c>
       <c r="D66" s="30" t="s">
         <v>79</v>
       </c>
@@ -5899,7 +5947,9 @@
       <c r="B67" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C67" s="29"/>
+      <c r="C67" s="42" t="s">
+        <v>291</v>
+      </c>
       <c r="D67" s="30" t="s">
         <v>78</v>
       </c>
@@ -6023,7 +6073,9 @@
       <c r="B70" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="C70" s="47"/>
+      <c r="C70" s="58" t="s">
+        <v>291</v>
+      </c>
       <c r="D70" s="48" t="s">
         <v>267</v>
       </c>
@@ -6494,574 +6546,201 @@
       <c r="AE80" s="15"/>
       <c r="AF80" s="17"/>
     </row>
-    <row r="81" spans="1:32" s="19" customFormat="1">
-      <c r="A81" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C81" s="11"/>
-      <c r="D81" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="E81" s="14">
-        <v>1</v>
-      </c>
-      <c r="F81" s="14">
-        <v>0</v>
-      </c>
-      <c r="G81" s="15">
-        <v>720</v>
-      </c>
-      <c r="H81" s="22"/>
-      <c r="I81" s="15">
-        <v>0</v>
-      </c>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="15"/>
-      <c r="V81" s="15"/>
-      <c r="W81" s="15"/>
-      <c r="X81" s="15"/>
-      <c r="Y81" s="15"/>
-      <c r="Z81" s="15"/>
-      <c r="AA81" s="15"/>
-      <c r="AB81" s="15"/>
-      <c r="AC81" s="15"/>
-      <c r="AD81" s="15"/>
-      <c r="AE81" s="15"/>
-      <c r="AF81" s="17"/>
-    </row>
-    <row r="82" spans="1:32" s="19" customFormat="1">
-      <c r="A82" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C82" s="11"/>
-      <c r="D82" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E82" s="20">
-        <v>1</v>
-      </c>
-      <c r="F82" s="21">
-        <v>0</v>
-      </c>
-      <c r="G82" s="18">
-        <v>360</v>
-      </c>
-      <c r="H82" s="22"/>
-      <c r="I82" s="18">
-        <v>0</v>
-      </c>
-      <c r="J82" s="15"/>
-      <c r="K82" s="15"/>
-      <c r="L82" s="15"/>
-      <c r="M82" s="15"/>
-      <c r="N82" s="15"/>
-      <c r="O82" s="15"/>
-      <c r="P82" s="15"/>
-      <c r="Q82" s="15"/>
-      <c r="R82" s="15"/>
-      <c r="S82" s="15"/>
-      <c r="T82" s="15"/>
-      <c r="U82" s="15"/>
-      <c r="V82" s="15"/>
-      <c r="W82" s="15"/>
-      <c r="X82" s="15"/>
-      <c r="Y82" s="15"/>
-      <c r="Z82" s="15"/>
-      <c r="AA82" s="15"/>
-      <c r="AB82" s="15"/>
-      <c r="AC82" s="15"/>
-      <c r="AD82" s="15"/>
-      <c r="AE82" s="15"/>
-      <c r="AF82" s="17"/>
-    </row>
-    <row r="83" spans="1:32" s="19" customFormat="1">
-      <c r="A83" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B83" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83" s="11"/>
-      <c r="D83" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E83" s="14">
-        <v>0</v>
-      </c>
-      <c r="F83" s="14">
-        <v>0</v>
-      </c>
-      <c r="G83" s="15">
-        <v>0</v>
-      </c>
-      <c r="H83" s="22"/>
-      <c r="I83" s="15">
-        <v>0</v>
-      </c>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="15"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="15"/>
-      <c r="O83" s="15"/>
-      <c r="P83" s="15"/>
-      <c r="Q83" s="15"/>
-      <c r="R83" s="15"/>
-      <c r="S83" s="15"/>
-      <c r="T83" s="15"/>
-      <c r="U83" s="15"/>
-      <c r="V83" s="15"/>
-      <c r="W83" s="15"/>
-      <c r="X83" s="15"/>
-      <c r="Y83" s="15"/>
-      <c r="Z83" s="15"/>
-      <c r="AA83" s="15"/>
-      <c r="AB83" s="15"/>
-      <c r="AC83" s="15"/>
-      <c r="AD83" s="15"/>
-      <c r="AE83" s="15"/>
-      <c r="AF83" s="17"/>
-    </row>
-    <row r="84" spans="1:32" s="19" customFormat="1">
-      <c r="A84" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B84" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C84" s="11"/>
-      <c r="D84" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E84" s="14">
-        <v>0</v>
-      </c>
-      <c r="F84" s="14">
-        <v>0</v>
-      </c>
-      <c r="G84" s="15">
-        <v>0</v>
-      </c>
-      <c r="H84" s="22"/>
-      <c r="I84" s="15">
-        <v>0</v>
-      </c>
-      <c r="J84" s="15"/>
-      <c r="K84" s="15"/>
-      <c r="L84" s="15"/>
-      <c r="M84" s="15"/>
-      <c r="N84" s="15"/>
-      <c r="O84" s="15"/>
-      <c r="P84" s="15"/>
-      <c r="Q84" s="15"/>
-      <c r="R84" s="15"/>
-      <c r="S84" s="15"/>
-      <c r="T84" s="15"/>
-      <c r="U84" s="15"/>
-      <c r="V84" s="15"/>
-      <c r="W84" s="15"/>
-      <c r="X84" s="15"/>
-      <c r="Y84" s="15"/>
-      <c r="Z84" s="15"/>
-      <c r="AA84" s="15"/>
-      <c r="AB84" s="15"/>
-      <c r="AC84" s="15"/>
-      <c r="AD84" s="15"/>
-      <c r="AE84" s="15"/>
-      <c r="AF84" s="17"/>
-    </row>
-    <row r="85" spans="1:32" s="19" customFormat="1">
-      <c r="A85" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C85" s="11"/>
-      <c r="D85" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E85" s="14">
-        <v>0</v>
-      </c>
-      <c r="F85" s="14">
-        <v>0</v>
-      </c>
-      <c r="G85" s="15">
-        <v>0</v>
-      </c>
-      <c r="H85" s="22"/>
-      <c r="I85" s="15">
-        <v>0</v>
-      </c>
-      <c r="J85" s="15"/>
-      <c r="K85" s="15"/>
-      <c r="L85" s="15"/>
-      <c r="M85" s="15"/>
-      <c r="N85" s="15"/>
-      <c r="O85" s="15"/>
-      <c r="P85" s="15"/>
-      <c r="Q85" s="15"/>
-      <c r="R85" s="15"/>
-      <c r="S85" s="15"/>
-      <c r="T85" s="15"/>
-      <c r="U85" s="15"/>
-      <c r="V85" s="15"/>
-      <c r="W85" s="15"/>
-      <c r="X85" s="15"/>
-      <c r="Y85" s="15"/>
-      <c r="Z85" s="15"/>
-      <c r="AA85" s="15"/>
-      <c r="AB85" s="15"/>
-      <c r="AC85" s="15"/>
-      <c r="AD85" s="15"/>
-      <c r="AE85" s="15"/>
-      <c r="AF85" s="17"/>
-    </row>
-    <row r="86" spans="1:32" s="19" customFormat="1">
-      <c r="A86" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B86" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C86" s="11"/>
-      <c r="D86" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E86" s="14">
-        <v>0</v>
-      </c>
-      <c r="F86" s="14">
-        <v>0</v>
-      </c>
-      <c r="G86" s="15">
-        <v>0</v>
-      </c>
-      <c r="H86" s="22"/>
-      <c r="I86" s="15">
-        <v>0</v>
-      </c>
-      <c r="J86" s="15"/>
-      <c r="K86" s="15"/>
-      <c r="L86" s="15"/>
-      <c r="M86" s="15"/>
-      <c r="N86" s="15"/>
-      <c r="O86" s="15"/>
-      <c r="P86" s="15"/>
-      <c r="Q86" s="15"/>
-      <c r="R86" s="15"/>
-      <c r="S86" s="15"/>
-      <c r="T86" s="15"/>
-      <c r="U86" s="15"/>
-      <c r="V86" s="15"/>
-      <c r="W86" s="15"/>
-      <c r="X86" s="15"/>
-      <c r="Y86" s="15"/>
-      <c r="Z86" s="15"/>
-      <c r="AA86" s="15"/>
-      <c r="AB86" s="15"/>
-      <c r="AC86" s="15"/>
-      <c r="AD86" s="15"/>
-      <c r="AE86" s="15"/>
-      <c r="AF86" s="17"/>
-    </row>
-    <row r="87" spans="1:32" s="19" customFormat="1">
-      <c r="A87" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C87" s="11"/>
-      <c r="D87" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" s="14">
-        <v>1</v>
-      </c>
-      <c r="F87" s="14">
-        <v>400</v>
-      </c>
-      <c r="G87" s="15">
-        <v>48</v>
-      </c>
-      <c r="H87" s="22"/>
-      <c r="I87" s="15">
-        <v>20</v>
-      </c>
-      <c r="J87" s="15"/>
-      <c r="K87" s="15"/>
-      <c r="L87" s="15"/>
-      <c r="M87" s="15"/>
-      <c r="N87" s="15"/>
-      <c r="O87" s="15"/>
-      <c r="P87" s="15"/>
-      <c r="Q87" s="15"/>
-      <c r="R87" s="15"/>
-      <c r="S87" s="15"/>
-      <c r="T87" s="15"/>
-      <c r="U87" s="15"/>
-      <c r="V87" s="15"/>
-      <c r="W87" s="15"/>
-      <c r="X87" s="15"/>
-      <c r="Y87" s="15"/>
-      <c r="Z87" s="15"/>
-      <c r="AA87" s="15"/>
-      <c r="AB87" s="15"/>
-      <c r="AC87" s="15"/>
-      <c r="AD87" s="15"/>
-      <c r="AE87" s="15"/>
-      <c r="AF87" s="17"/>
-    </row>
-    <row r="88" spans="1:32" s="19" customFormat="1">
-      <c r="A88" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C88" s="11"/>
-      <c r="D88" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E88" s="14">
-        <v>1</v>
-      </c>
-      <c r="F88" s="14">
-        <v>400</v>
-      </c>
-      <c r="G88" s="15">
-        <v>48</v>
-      </c>
-      <c r="H88" s="22"/>
-      <c r="I88" s="15">
-        <v>40</v>
-      </c>
-      <c r="J88" s="15"/>
-      <c r="K88" s="15"/>
-      <c r="L88" s="15"/>
-      <c r="M88" s="15"/>
-      <c r="N88" s="15"/>
-      <c r="O88" s="15"/>
-      <c r="P88" s="15"/>
-      <c r="Q88" s="15"/>
-      <c r="R88" s="15"/>
-      <c r="S88" s="15"/>
-      <c r="T88" s="15"/>
-      <c r="U88" s="15"/>
-      <c r="V88" s="15"/>
-      <c r="W88" s="15"/>
-      <c r="X88" s="15"/>
-      <c r="Y88" s="15"/>
-      <c r="Z88" s="15"/>
-      <c r="AA88" s="15"/>
-      <c r="AB88" s="15"/>
-      <c r="AC88" s="15"/>
-      <c r="AD88" s="15"/>
-      <c r="AE88" s="15"/>
-      <c r="AF88" s="17"/>
-    </row>
-    <row r="89" spans="1:32" s="19" customFormat="1">
-      <c r="A89" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C89" s="11"/>
-      <c r="D89" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="E89" s="20">
-        <v>0</v>
-      </c>
-      <c r="F89" s="21">
-        <v>0</v>
-      </c>
-      <c r="G89" s="18">
-        <v>0</v>
-      </c>
-      <c r="H89" s="22"/>
-      <c r="I89" s="18">
-        <v>0</v>
-      </c>
-      <c r="J89" s="15"/>
-      <c r="K89" s="15"/>
-      <c r="L89" s="15"/>
-      <c r="M89" s="15"/>
-      <c r="N89" s="15"/>
-      <c r="O89" s="15"/>
-      <c r="P89" s="15"/>
-      <c r="Q89" s="15"/>
-      <c r="R89" s="15"/>
-      <c r="S89" s="15"/>
-      <c r="T89" s="15"/>
-      <c r="U89" s="15"/>
-      <c r="V89" s="15"/>
-      <c r="W89" s="15"/>
-      <c r="X89" s="15"/>
-      <c r="Y89" s="15"/>
-      <c r="Z89" s="15"/>
-      <c r="AA89" s="15"/>
-      <c r="AB89" s="15"/>
-      <c r="AC89" s="15"/>
-      <c r="AD89" s="15"/>
-      <c r="AE89" s="15"/>
-      <c r="AF89" s="17"/>
-    </row>
-    <row r="90" spans="1:32" s="19" customFormat="1">
-      <c r="A90" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="E90" s="20"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="22"/>
-      <c r="I90" s="15"/>
-      <c r="J90" s="15"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="15"/>
-      <c r="M90" s="15"/>
-      <c r="N90" s="15"/>
-      <c r="O90" s="15"/>
-      <c r="P90" s="15"/>
-      <c r="Q90" s="15"/>
-      <c r="R90" s="15"/>
-      <c r="S90" s="15"/>
-      <c r="T90" s="15"/>
-      <c r="U90" s="15"/>
-      <c r="V90" s="15"/>
-      <c r="W90" s="15"/>
-      <c r="X90" s="15"/>
-      <c r="Y90" s="15"/>
-      <c r="Z90" s="15"/>
-      <c r="AA90" s="15"/>
-      <c r="AB90" s="15"/>
-      <c r="AC90" s="15"/>
-      <c r="AD90" s="15"/>
-      <c r="AE90" s="15"/>
-      <c r="AF90" s="17"/>
-    </row>
-    <row r="91" spans="1:32" s="19" customFormat="1">
-      <c r="A91" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="C91" s="11"/>
-      <c r="D91" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E91" s="20"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="22"/>
-      <c r="I91" s="15"/>
-      <c r="J91" s="15"/>
-      <c r="K91" s="15"/>
-      <c r="L91" s="15"/>
-      <c r="M91" s="15"/>
-      <c r="N91" s="15"/>
-      <c r="O91" s="15"/>
-      <c r="P91" s="15"/>
-      <c r="Q91" s="15"/>
-      <c r="R91" s="15"/>
-      <c r="S91" s="15"/>
-      <c r="T91" s="15"/>
-      <c r="U91" s="15"/>
-      <c r="V91" s="15"/>
-      <c r="W91" s="15"/>
-      <c r="X91" s="15"/>
-      <c r="Y91" s="15"/>
-      <c r="Z91" s="15"/>
-      <c r="AA91" s="15"/>
-      <c r="AB91" s="15"/>
-      <c r="AC91" s="15"/>
-      <c r="AD91" s="15"/>
-      <c r="AE91" s="15"/>
-      <c r="AF91" s="17"/>
-    </row>
-    <row r="92" spans="1:32" s="19" customFormat="1">
-      <c r="A92" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="E92" s="20"/>
-      <c r="F92" s="21"/>
-      <c r="G92" s="18"/>
-      <c r="H92" s="22"/>
-      <c r="I92" s="15"/>
-      <c r="J92" s="15"/>
-      <c r="K92" s="15"/>
-      <c r="L92" s="15"/>
-      <c r="M92" s="15"/>
-      <c r="N92" s="15"/>
-      <c r="O92" s="15"/>
-      <c r="P92" s="15"/>
-      <c r="Q92" s="15"/>
-      <c r="R92" s="15"/>
-      <c r="S92" s="15"/>
-      <c r="T92" s="15"/>
-      <c r="U92" s="15"/>
-      <c r="V92" s="15"/>
-      <c r="W92" s="15"/>
-      <c r="X92" s="15"/>
-      <c r="Y92" s="15"/>
-      <c r="Z92" s="15"/>
-      <c r="AA92" s="15"/>
-      <c r="AB92" s="15"/>
-      <c r="AC92" s="15"/>
-      <c r="AD92" s="15"/>
-      <c r="AE92" s="15"/>
-      <c r="AF92" s="17"/>
+    <row r="81" spans="1:32" s="55" customFormat="1">
+      <c r="A81" s="56" t="s">
+        <v>275</v>
+      </c>
+      <c r="B81" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="C81" s="56"/>
+      <c r="D81" s="64" t="s">
+        <v>282</v>
+      </c>
+      <c r="E81" s="61"/>
+      <c r="F81" s="61"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="63"/>
+      <c r="I81" s="62"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="62"/>
+      <c r="L81" s="62"/>
+      <c r="M81" s="62"/>
+      <c r="N81" s="62"/>
+      <c r="O81" s="62"/>
+      <c r="P81" s="62"/>
+      <c r="Q81" s="62"/>
+      <c r="R81" s="62"/>
+      <c r="S81" s="62"/>
+      <c r="T81" s="62"/>
+      <c r="U81" s="62"/>
+      <c r="V81" s="62"/>
+      <c r="W81" s="62"/>
+      <c r="X81" s="62"/>
+      <c r="Y81" s="62"/>
+      <c r="Z81" s="62"/>
+      <c r="AA81" s="62"/>
+      <c r="AB81" s="62"/>
+      <c r="AC81" s="62"/>
+      <c r="AD81" s="62"/>
+      <c r="AE81" s="62"/>
+      <c r="AF81" s="62"/>
+    </row>
+    <row r="82" spans="1:32" s="55" customFormat="1">
+      <c r="A82" s="56" t="s">
+        <v>275</v>
+      </c>
+      <c r="B82" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="C82" s="56"/>
+      <c r="D82" s="64" t="s">
+        <v>281</v>
+      </c>
+      <c r="E82" s="61"/>
+      <c r="F82" s="61"/>
+      <c r="G82" s="62"/>
+      <c r="H82" s="63"/>
+      <c r="I82" s="62"/>
+      <c r="J82" s="62"/>
+      <c r="K82" s="62"/>
+      <c r="L82" s="62"/>
+      <c r="M82" s="62"/>
+      <c r="N82" s="62"/>
+      <c r="O82" s="62"/>
+      <c r="P82" s="62"/>
+      <c r="Q82" s="62"/>
+      <c r="R82" s="62"/>
+      <c r="S82" s="62"/>
+      <c r="T82" s="62"/>
+      <c r="U82" s="62"/>
+      <c r="V82" s="62"/>
+      <c r="W82" s="62"/>
+      <c r="X82" s="62"/>
+      <c r="Y82" s="62"/>
+      <c r="Z82" s="62"/>
+      <c r="AA82" s="62"/>
+      <c r="AB82" s="62"/>
+      <c r="AC82" s="62"/>
+      <c r="AD82" s="62"/>
+      <c r="AE82" s="62"/>
+      <c r="AF82" s="62"/>
+    </row>
+    <row r="83" spans="1:32" s="55" customFormat="1">
+      <c r="A83" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="B83" s="55" t="s">
+        <v>277</v>
+      </c>
+      <c r="D83" s="64" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="84" spans="1:32" s="55" customFormat="1">
+      <c r="A84" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="B84" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="D84" s="64" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="85" spans="1:32" s="55" customFormat="1">
+      <c r="A85" s="56" t="s">
+        <v>285</v>
+      </c>
+      <c r="D85" s="64"/>
+    </row>
+    <row r="86" spans="1:32" s="55" customFormat="1">
+      <c r="A86" s="56" t="s">
+        <v>285</v>
+      </c>
+      <c r="D86" s="64"/>
+    </row>
+    <row r="87" spans="1:32" s="55" customFormat="1">
+      <c r="A87" s="56" t="s">
+        <v>286</v>
+      </c>
+      <c r="B87" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="D87" s="64" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="88" spans="1:32" s="55" customFormat="1">
+      <c r="A88" s="56" t="s">
+        <v>286</v>
+      </c>
+      <c r="B88" s="55" t="s">
+        <v>287</v>
+      </c>
+      <c r="D88" s="64" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="89" spans="1:32" s="35" customFormat="1">
+      <c r="A89" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="B89" s="47"/>
+      <c r="D89" s="65"/>
+    </row>
+    <row r="90" spans="1:32" s="35" customFormat="1">
+      <c r="A90" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="D90" s="65"/>
+    </row>
+    <row r="91" spans="1:32" s="35" customFormat="1">
+      <c r="A91" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="B91" s="66" t="s">
+        <v>294</v>
+      </c>
+      <c r="D91" s="67" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="92" spans="1:32" s="35" customFormat="1">
+      <c r="A92" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="B92" s="66" t="s">
+        <v>295</v>
+      </c>
+      <c r="D92" s="67" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="93" spans="1:32" s="19" customFormat="1">
       <c r="A93" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
       <c r="C93" s="11"/>
       <c r="D93" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E93" s="20"/>
-      <c r="F93" s="21"/>
-      <c r="G93" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="E93" s="14">
+        <v>1</v>
+      </c>
+      <c r="F93" s="14">
+        <v>400</v>
+      </c>
+      <c r="G93" s="15">
+        <v>48</v>
+      </c>
       <c r="H93" s="22"/>
-      <c r="I93" s="15"/>
+      <c r="I93" s="15">
+        <v>20</v>
+      </c>
       <c r="J93" s="15"/>
       <c r="K93" s="15"/>
       <c r="L93" s="15"/>
@@ -7088,20 +6767,28 @@
     </row>
     <row r="94" spans="1:32" s="19" customFormat="1">
       <c r="A94" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="C94" s="11"/>
       <c r="D94" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="E94" s="20"/>
-      <c r="F94" s="21"/>
-      <c r="G94" s="18"/>
+        <v>34</v>
+      </c>
+      <c r="E94" s="14">
+        <v>1</v>
+      </c>
+      <c r="F94" s="14">
+        <v>400</v>
+      </c>
+      <c r="G94" s="15">
+        <v>48</v>
+      </c>
       <c r="H94" s="22"/>
-      <c r="I94" s="15"/>
+      <c r="I94" s="15">
+        <v>40</v>
+      </c>
       <c r="J94" s="15"/>
       <c r="K94" s="15"/>
       <c r="L94" s="15"/>
@@ -7128,14 +6815,14 @@
     </row>
     <row r="95" spans="1:32" s="19" customFormat="1">
       <c r="A95" s="11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="12" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="E95" s="20">
         <v>0</v>
@@ -7147,7 +6834,7 @@
         <v>0</v>
       </c>
       <c r="H95" s="22"/>
-      <c r="I95" s="15">
+      <c r="I95" s="18">
         <v>0</v>
       </c>
       <c r="J95" s="15"/>
@@ -7179,25 +6866,17 @@
         <v>36</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>181</v>
+        <v>203</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E96" s="20">
-        <v>0</v>
-      </c>
-      <c r="F96" s="21">
-        <v>0</v>
-      </c>
-      <c r="G96" s="18">
-        <v>0</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="E96" s="20"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="18"/>
       <c r="H96" s="22"/>
-      <c r="I96" s="15">
-        <v>0</v>
-      </c>
+      <c r="I96" s="15"/>
       <c r="J96" s="15"/>
       <c r="K96" s="15"/>
       <c r="L96" s="15"/>
@@ -7223,29 +6902,21 @@
       <c r="AF96" s="17"/>
     </row>
     <row r="97" spans="1:32" s="19" customFormat="1">
-      <c r="A97" s="57" t="s">
+      <c r="A97" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="C97" s="11"/>
       <c r="D97" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="E97" s="20">
-        <v>0</v>
-      </c>
-      <c r="F97" s="21">
-        <v>0</v>
-      </c>
-      <c r="G97" s="18">
-        <v>0</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="E97" s="20"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="18"/>
       <c r="H97" s="22"/>
-      <c r="I97" s="15">
-        <v>0</v>
-      </c>
+      <c r="I97" s="15"/>
       <c r="J97" s="15"/>
       <c r="K97" s="15"/>
       <c r="L97" s="15"/>
@@ -7271,154 +6942,594 @@
       <c r="AF97" s="17"/>
     </row>
     <row r="98" spans="1:32" s="19" customFormat="1">
-      <c r="A98" s="60"/>
-      <c r="B98" s="23" t="s">
+      <c r="A98" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E98" s="20"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="22"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="15"/>
+      <c r="O98" s="15"/>
+      <c r="P98" s="15"/>
+      <c r="Q98" s="15"/>
+      <c r="R98" s="15"/>
+      <c r="S98" s="15"/>
+      <c r="T98" s="15"/>
+      <c r="U98" s="15"/>
+      <c r="V98" s="15"/>
+      <c r="W98" s="15"/>
+      <c r="X98" s="15"/>
+      <c r="Y98" s="15"/>
+      <c r="Z98" s="15"/>
+      <c r="AA98" s="15"/>
+      <c r="AB98" s="15"/>
+      <c r="AC98" s="15"/>
+      <c r="AD98" s="15"/>
+      <c r="AE98" s="15"/>
+      <c r="AF98" s="17"/>
+    </row>
+    <row r="99" spans="1:32" s="19" customFormat="1">
+      <c r="A99" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E99" s="20"/>
+      <c r="F99" s="21"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15"/>
+      <c r="L99" s="15"/>
+      <c r="M99" s="15"/>
+      <c r="N99" s="15"/>
+      <c r="O99" s="15"/>
+      <c r="P99" s="15"/>
+      <c r="Q99" s="15"/>
+      <c r="R99" s="15"/>
+      <c r="S99" s="15"/>
+      <c r="T99" s="15"/>
+      <c r="U99" s="15"/>
+      <c r="V99" s="15"/>
+      <c r="W99" s="15"/>
+      <c r="X99" s="15"/>
+      <c r="Y99" s="15"/>
+      <c r="Z99" s="15"/>
+      <c r="AA99" s="15"/>
+      <c r="AB99" s="15"/>
+      <c r="AC99" s="15"/>
+      <c r="AD99" s="15"/>
+      <c r="AE99" s="15"/>
+      <c r="AF99" s="17"/>
+    </row>
+    <row r="100" spans="1:32" s="19" customFormat="1">
+      <c r="A100" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B100" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C100" s="11"/>
+      <c r="D100" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E100" s="20"/>
+      <c r="F100" s="21"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="15"/>
+      <c r="L100" s="15"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="15"/>
+      <c r="O100" s="15"/>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="15"/>
+      <c r="R100" s="15"/>
+      <c r="S100" s="15"/>
+      <c r="T100" s="15"/>
+      <c r="U100" s="15"/>
+      <c r="V100" s="15"/>
+      <c r="W100" s="15"/>
+      <c r="X100" s="15"/>
+      <c r="Y100" s="15"/>
+      <c r="Z100" s="15"/>
+      <c r="AA100" s="15"/>
+      <c r="AB100" s="15"/>
+      <c r="AC100" s="15"/>
+      <c r="AD100" s="15"/>
+      <c r="AE100" s="15"/>
+      <c r="AF100" s="17"/>
+    </row>
+    <row r="101" spans="1:32" s="19" customFormat="1">
+      <c r="A101" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C101" s="11"/>
+      <c r="D101" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E101" s="20">
+        <v>0</v>
+      </c>
+      <c r="F101" s="21">
+        <v>0</v>
+      </c>
+      <c r="G101" s="18">
+        <v>0</v>
+      </c>
+      <c r="H101" s="22"/>
+      <c r="I101" s="15">
+        <v>0</v>
+      </c>
+      <c r="J101" s="15"/>
+      <c r="K101" s="15"/>
+      <c r="L101" s="15"/>
+      <c r="M101" s="15"/>
+      <c r="N101" s="15"/>
+      <c r="O101" s="15"/>
+      <c r="P101" s="15"/>
+      <c r="Q101" s="15"/>
+      <c r="R101" s="15"/>
+      <c r="S101" s="15"/>
+      <c r="T101" s="15"/>
+      <c r="U101" s="15"/>
+      <c r="V101" s="15"/>
+      <c r="W101" s="15"/>
+      <c r="X101" s="15"/>
+      <c r="Y101" s="15"/>
+      <c r="Z101" s="15"/>
+      <c r="AA101" s="15"/>
+      <c r="AB101" s="15"/>
+      <c r="AC101" s="15"/>
+      <c r="AD101" s="15"/>
+      <c r="AE101" s="15"/>
+      <c r="AF101" s="17"/>
+    </row>
+    <row r="102" spans="1:32" s="19" customFormat="1">
+      <c r="A102" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C102" s="11"/>
+      <c r="D102" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="E102" s="20">
+        <v>0</v>
+      </c>
+      <c r="F102" s="21">
+        <v>0</v>
+      </c>
+      <c r="G102" s="18">
+        <v>0</v>
+      </c>
+      <c r="H102" s="22"/>
+      <c r="I102" s="15">
+        <v>0</v>
+      </c>
+      <c r="J102" s="15"/>
+      <c r="K102" s="15"/>
+      <c r="L102" s="15"/>
+      <c r="M102" s="15"/>
+      <c r="N102" s="15"/>
+      <c r="O102" s="15"/>
+      <c r="P102" s="15"/>
+      <c r="Q102" s="15"/>
+      <c r="R102" s="15"/>
+      <c r="S102" s="15"/>
+      <c r="T102" s="15"/>
+      <c r="U102" s="15"/>
+      <c r="V102" s="15"/>
+      <c r="W102" s="15"/>
+      <c r="X102" s="15"/>
+      <c r="Y102" s="15"/>
+      <c r="Z102" s="15"/>
+      <c r="AA102" s="15"/>
+      <c r="AB102" s="15"/>
+      <c r="AC102" s="15"/>
+      <c r="AD102" s="15"/>
+      <c r="AE102" s="15"/>
+      <c r="AF102" s="17"/>
+    </row>
+    <row r="103" spans="1:32" s="19" customFormat="1">
+      <c r="A103" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C103" s="11"/>
+      <c r="D103" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E103" s="20">
+        <v>0</v>
+      </c>
+      <c r="F103" s="21">
+        <v>0</v>
+      </c>
+      <c r="G103" s="18">
+        <v>0</v>
+      </c>
+      <c r="H103" s="22"/>
+      <c r="I103" s="15">
+        <v>0</v>
+      </c>
+      <c r="J103" s="15"/>
+      <c r="K103" s="15"/>
+      <c r="L103" s="15"/>
+      <c r="M103" s="15"/>
+      <c r="N103" s="15"/>
+      <c r="O103" s="15"/>
+      <c r="P103" s="15"/>
+      <c r="Q103" s="15"/>
+      <c r="R103" s="15"/>
+      <c r="S103" s="15"/>
+      <c r="T103" s="15"/>
+      <c r="U103" s="15"/>
+      <c r="V103" s="15"/>
+      <c r="W103" s="15"/>
+      <c r="X103" s="15"/>
+      <c r="Y103" s="15"/>
+      <c r="Z103" s="15"/>
+      <c r="AA103" s="15"/>
+      <c r="AB103" s="15"/>
+      <c r="AC103" s="15"/>
+      <c r="AD103" s="15"/>
+      <c r="AE103" s="15"/>
+      <c r="AF103" s="17"/>
+    </row>
+    <row r="104" spans="1:32" s="19" customFormat="1">
+      <c r="A104" s="60"/>
+      <c r="B104" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="C98" s="23"/>
-      <c r="D98" s="24" t="s">
+      <c r="C104" s="23"/>
+      <c r="D104" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="23"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
-      <c r="O98" s="27"/>
-      <c r="P98" s="27"/>
-      <c r="Q98" s="27"/>
-      <c r="R98" s="27"/>
-      <c r="S98" s="27"/>
-      <c r="T98" s="27"/>
-      <c r="U98" s="27"/>
-      <c r="V98" s="27"/>
-      <c r="W98" s="27"/>
-      <c r="X98" s="27"/>
-      <c r="Y98" s="27"/>
-      <c r="Z98" s="27"/>
-      <c r="AA98" s="27"/>
-      <c r="AB98" s="27"/>
-      <c r="AC98" s="27"/>
-      <c r="AD98" s="27"/>
-      <c r="AE98" s="27"/>
-      <c r="AF98" s="28"/>
-    </row>
-    <row r="99" spans="1:32" s="55" customFormat="1">
-      <c r="A99" s="56" t="s">
-        <v>275</v>
-      </c>
-      <c r="B99" s="56" t="s">
-        <v>279</v>
-      </c>
-      <c r="C99" s="56"/>
-      <c r="D99" s="64" t="s">
-        <v>282</v>
-      </c>
-      <c r="E99" s="61"/>
-      <c r="F99" s="61"/>
-      <c r="G99" s="62"/>
-      <c r="H99" s="63"/>
-      <c r="I99" s="62"/>
-      <c r="J99" s="62"/>
-      <c r="K99" s="62"/>
-      <c r="L99" s="62"/>
-      <c r="M99" s="62"/>
-      <c r="N99" s="62"/>
-      <c r="O99" s="62"/>
-      <c r="P99" s="62"/>
-      <c r="Q99" s="62"/>
-      <c r="R99" s="62"/>
-      <c r="S99" s="62"/>
-      <c r="T99" s="62"/>
-      <c r="U99" s="62"/>
-      <c r="V99" s="62"/>
-      <c r="W99" s="62"/>
-      <c r="X99" s="62"/>
-      <c r="Y99" s="62"/>
-      <c r="Z99" s="62"/>
-      <c r="AA99" s="62"/>
-      <c r="AB99" s="62"/>
-      <c r="AC99" s="62"/>
-      <c r="AD99" s="62"/>
-      <c r="AE99" s="62"/>
-      <c r="AF99" s="62"/>
-    </row>
-    <row r="100" spans="1:32" s="55" customFormat="1">
-      <c r="A100" s="56" t="s">
-        <v>275</v>
-      </c>
-      <c r="B100" s="56" t="s">
-        <v>280</v>
-      </c>
-      <c r="C100" s="56"/>
-      <c r="D100" s="64" t="s">
-        <v>281</v>
-      </c>
-      <c r="E100" s="61"/>
-      <c r="F100" s="61"/>
-      <c r="G100" s="62"/>
-      <c r="H100" s="63"/>
-      <c r="I100" s="62"/>
-      <c r="J100" s="62"/>
-      <c r="K100" s="62"/>
-      <c r="L100" s="62"/>
-      <c r="M100" s="62"/>
-      <c r="N100" s="62"/>
-      <c r="O100" s="62"/>
-      <c r="P100" s="62"/>
-      <c r="Q100" s="62"/>
-      <c r="R100" s="62"/>
-      <c r="S100" s="62"/>
-      <c r="T100" s="62"/>
-      <c r="U100" s="62"/>
-      <c r="V100" s="62"/>
-      <c r="W100" s="62"/>
-      <c r="X100" s="62"/>
-      <c r="Y100" s="62"/>
-      <c r="Z100" s="62"/>
-      <c r="AA100" s="62"/>
-      <c r="AB100" s="62"/>
-      <c r="AC100" s="62"/>
-      <c r="AD100" s="62"/>
-      <c r="AE100" s="62"/>
-      <c r="AF100" s="62"/>
-    </row>
-    <row r="101" spans="1:32" s="55" customFormat="1">
-      <c r="A101" s="56" t="s">
-        <v>276</v>
-      </c>
-      <c r="B101" s="55" t="s">
-        <v>277</v>
-      </c>
-      <c r="D101" s="64" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="102" spans="1:32" s="55" customFormat="1">
-      <c r="A102" s="56" t="s">
-        <v>276</v>
-      </c>
-      <c r="B102" s="55" t="s">
-        <v>278</v>
-      </c>
-      <c r="D102" s="64" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="103" spans="1:32">
-      <c r="A103" s="65" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="104" spans="1:32">
-      <c r="A104" s="65" t="s">
-        <v>285</v>
-      </c>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="26"/>
+      <c r="I104" s="27"/>
+      <c r="J104" s="27"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="27"/>
+      <c r="M104" s="27"/>
+      <c r="N104" s="27"/>
+      <c r="O104" s="27"/>
+      <c r="P104" s="27"/>
+      <c r="Q104" s="27"/>
+      <c r="R104" s="27"/>
+      <c r="S104" s="27"/>
+      <c r="T104" s="27"/>
+      <c r="U104" s="27"/>
+      <c r="V104" s="27"/>
+      <c r="W104" s="27"/>
+      <c r="X104" s="27"/>
+      <c r="Y104" s="27"/>
+      <c r="Z104" s="27"/>
+      <c r="AA104" s="27"/>
+      <c r="AB104" s="27"/>
+      <c r="AC104" s="27"/>
+      <c r="AD104" s="27"/>
+      <c r="AE104" s="27"/>
+      <c r="AF104" s="28"/>
+    </row>
+    <row r="105" spans="1:32" s="19" customFormat="1">
+      <c r="A105" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E105" s="14">
+        <v>1</v>
+      </c>
+      <c r="F105" s="14">
+        <v>0</v>
+      </c>
+      <c r="G105" s="15">
+        <v>720</v>
+      </c>
+      <c r="H105" s="22"/>
+      <c r="I105" s="15">
+        <v>0</v>
+      </c>
+      <c r="J105" s="15"/>
+      <c r="K105" s="15"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="15"/>
+      <c r="N105" s="15"/>
+      <c r="O105" s="15"/>
+      <c r="P105" s="15"/>
+      <c r="Q105" s="15"/>
+      <c r="R105" s="15"/>
+      <c r="S105" s="15"/>
+      <c r="T105" s="15"/>
+      <c r="U105" s="15"/>
+      <c r="V105" s="15"/>
+      <c r="W105" s="15"/>
+      <c r="X105" s="15"/>
+      <c r="Y105" s="15"/>
+      <c r="Z105" s="15"/>
+      <c r="AA105" s="15"/>
+      <c r="AB105" s="15"/>
+      <c r="AC105" s="15"/>
+      <c r="AD105" s="15"/>
+      <c r="AE105" s="15"/>
+      <c r="AF105" s="17"/>
+    </row>
+    <row r="106" spans="1:32" s="19" customFormat="1">
+      <c r="A106" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C106" s="11"/>
+      <c r="D106" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E106" s="20">
+        <v>1</v>
+      </c>
+      <c r="F106" s="21">
+        <v>0</v>
+      </c>
+      <c r="G106" s="18">
+        <v>360</v>
+      </c>
+      <c r="H106" s="22"/>
+      <c r="I106" s="18">
+        <v>0</v>
+      </c>
+      <c r="J106" s="15"/>
+      <c r="K106" s="15"/>
+      <c r="L106" s="15"/>
+      <c r="M106" s="15"/>
+      <c r="N106" s="15"/>
+      <c r="O106" s="15"/>
+      <c r="P106" s="15"/>
+      <c r="Q106" s="15"/>
+      <c r="R106" s="15"/>
+      <c r="S106" s="15"/>
+      <c r="T106" s="15"/>
+      <c r="U106" s="15"/>
+      <c r="V106" s="15"/>
+      <c r="W106" s="15"/>
+      <c r="X106" s="15"/>
+      <c r="Y106" s="15"/>
+      <c r="Z106" s="15"/>
+      <c r="AA106" s="15"/>
+      <c r="AB106" s="15"/>
+      <c r="AC106" s="15"/>
+      <c r="AD106" s="15"/>
+      <c r="AE106" s="15"/>
+      <c r="AF106" s="17"/>
+    </row>
+    <row r="107" spans="1:32" s="19" customFormat="1">
+      <c r="A107" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" s="11"/>
+      <c r="D107" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E107" s="14">
+        <v>0</v>
+      </c>
+      <c r="F107" s="14">
+        <v>0</v>
+      </c>
+      <c r="G107" s="15">
+        <v>0</v>
+      </c>
+      <c r="H107" s="22"/>
+      <c r="I107" s="15">
+        <v>0</v>
+      </c>
+      <c r="J107" s="15"/>
+      <c r="K107" s="15"/>
+      <c r="L107" s="15"/>
+      <c r="M107" s="15"/>
+      <c r="N107" s="15"/>
+      <c r="O107" s="15"/>
+      <c r="P107" s="15"/>
+      <c r="Q107" s="15"/>
+      <c r="R107" s="15"/>
+      <c r="S107" s="15"/>
+      <c r="T107" s="15"/>
+      <c r="U107" s="15"/>
+      <c r="V107" s="15"/>
+      <c r="W107" s="15"/>
+      <c r="X107" s="15"/>
+      <c r="Y107" s="15"/>
+      <c r="Z107" s="15"/>
+      <c r="AA107" s="15"/>
+      <c r="AB107" s="15"/>
+      <c r="AC107" s="15"/>
+      <c r="AD107" s="15"/>
+      <c r="AE107" s="15"/>
+      <c r="AF107" s="17"/>
+    </row>
+    <row r="108" spans="1:32" s="19" customFormat="1">
+      <c r="A108" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E108" s="14">
+        <v>0</v>
+      </c>
+      <c r="F108" s="14">
+        <v>0</v>
+      </c>
+      <c r="G108" s="15">
+        <v>0</v>
+      </c>
+      <c r="H108" s="22"/>
+      <c r="I108" s="15">
+        <v>0</v>
+      </c>
+      <c r="J108" s="15"/>
+      <c r="K108" s="15"/>
+      <c r="L108" s="15"/>
+      <c r="M108" s="15"/>
+      <c r="N108" s="15"/>
+      <c r="O108" s="15"/>
+      <c r="P108" s="15"/>
+      <c r="Q108" s="15"/>
+      <c r="R108" s="15"/>
+      <c r="S108" s="15"/>
+      <c r="T108" s="15"/>
+      <c r="U108" s="15"/>
+      <c r="V108" s="15"/>
+      <c r="W108" s="15"/>
+      <c r="X108" s="15"/>
+      <c r="Y108" s="15"/>
+      <c r="Z108" s="15"/>
+      <c r="AA108" s="15"/>
+      <c r="AB108" s="15"/>
+      <c r="AC108" s="15"/>
+      <c r="AD108" s="15"/>
+      <c r="AE108" s="15"/>
+      <c r="AF108" s="17"/>
+    </row>
+    <row r="109" spans="1:32" s="19" customFormat="1">
+      <c r="A109" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E109" s="14">
+        <v>0</v>
+      </c>
+      <c r="F109" s="14">
+        <v>0</v>
+      </c>
+      <c r="G109" s="15">
+        <v>0</v>
+      </c>
+      <c r="H109" s="22"/>
+      <c r="I109" s="15">
+        <v>0</v>
+      </c>
+      <c r="J109" s="15"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="15"/>
+      <c r="M109" s="15"/>
+      <c r="N109" s="15"/>
+      <c r="O109" s="15"/>
+      <c r="P109" s="15"/>
+      <c r="Q109" s="15"/>
+      <c r="R109" s="15"/>
+      <c r="S109" s="15"/>
+      <c r="T109" s="15"/>
+      <c r="U109" s="15"/>
+      <c r="V109" s="15"/>
+      <c r="W109" s="15"/>
+      <c r="X109" s="15"/>
+      <c r="Y109" s="15"/>
+      <c r="Z109" s="15"/>
+      <c r="AA109" s="15"/>
+      <c r="AB109" s="15"/>
+      <c r="AC109" s="15"/>
+      <c r="AD109" s="15"/>
+      <c r="AE109" s="15"/>
+      <c r="AF109" s="17"/>
+    </row>
+    <row r="110" spans="1:32" s="19" customFormat="1">
+      <c r="A110" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C110" s="11"/>
+      <c r="D110" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E110" s="14">
+        <v>0</v>
+      </c>
+      <c r="F110" s="14">
+        <v>0</v>
+      </c>
+      <c r="G110" s="15">
+        <v>0</v>
+      </c>
+      <c r="H110" s="22"/>
+      <c r="I110" s="15">
+        <v>0</v>
+      </c>
+      <c r="J110" s="15"/>
+      <c r="K110" s="15"/>
+      <c r="L110" s="15"/>
+      <c r="M110" s="15"/>
+      <c r="N110" s="15"/>
+      <c r="O110" s="15"/>
+      <c r="P110" s="15"/>
+      <c r="Q110" s="15"/>
+      <c r="R110" s="15"/>
+      <c r="S110" s="15"/>
+      <c r="T110" s="15"/>
+      <c r="U110" s="15"/>
+      <c r="V110" s="15"/>
+      <c r="W110" s="15"/>
+      <c r="X110" s="15"/>
+      <c r="Y110" s="15"/>
+      <c r="Z110" s="15"/>
+      <c r="AA110" s="15"/>
+      <c r="AB110" s="15"/>
+      <c r="AC110" s="15"/>
+      <c r="AD110" s="15"/>
+      <c r="AE110" s="15"/>
+      <c r="AF110" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
spawn point disappears when killed
</commit_message>
<xml_diff>
--- a/_xml/Abilities.xlsx
+++ b/_xml/Abilities.xlsx
@@ -2643,9 +2643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G32" sqref="G32"/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3049,8 +3049,8 @@
       <c r="B8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>148</v>
+      <c r="C8" s="39" t="s">
+        <v>229</v>
       </c>
       <c r="D8" s="40" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
Recycling/reusing icons. CY2 icons added.
</commit_message>
<xml_diff>
--- a/_xml/Abilities.xlsx
+++ b/_xml/Abilities.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="16155" windowHeight="8445"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -754,13 +754,28 @@
   </si>
   <si>
     <t>Sends forth bursts of solar energy.</t>
+  </si>
+  <si>
+    <t>Atiuh C.</t>
+  </si>
+  <si>
+    <t>Heat Body</t>
+  </si>
+  <si>
+    <t>Dashes in a line with emanating fire.</t>
+  </si>
+  <si>
+    <t>Rises into the air for a few seconds and then dives down, creating a shockwave.</t>
+  </si>
+  <si>
+    <t>Rising Sun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -978,7 +993,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1112,6 +1127,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1121,7 +1137,7 @@
   <dxfs count="35">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1135,7 +1151,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1151,7 +1167,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1167,7 +1183,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1183,7 +1199,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1199,7 +1215,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1215,7 +1231,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1231,7 +1247,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1247,7 +1263,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1263,7 +1279,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1279,7 +1295,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1295,7 +1311,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1311,7 +1327,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1327,7 +1343,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1343,7 +1359,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1359,7 +1375,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1375,7 +1391,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1391,7 +1407,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1407,7 +1423,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1423,7 +1439,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1439,7 +1455,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1455,7 +1471,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1471,7 +1487,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1487,7 +1503,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1503,7 +1519,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1519,7 +1535,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -1536,7 +1552,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -1551,7 +1567,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1565,7 +1581,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1620,7 +1636,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2258,7 +2274,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B2:AF72" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" dataCellStyle="20% - Accent1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="B2:AF74" tableType="xml" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" dataCellStyle="20% - Accent1">
   <tableColumns count="31">
     <tableColumn id="1" uniqueName="Name" name="Name" dataDxfId="30" dataCellStyle="20% - Accent1">
       <xmlColumnPr mapId="45" xpath="/Abilities/Ability/Name" xmlDataType="string"/>
@@ -2431,6 +2447,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2465,6 +2482,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2640,15 +2658,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F34" sqref="F34"/>
+      <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
@@ -2685,7 +2703,7 @@
     <col min="33" max="33" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -2696,7 +2714,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15.75" thickBot="1">
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2794,7 +2812,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="32" customFormat="1" ht="15.75" thickTop="1">
+    <row r="3" spans="1:32" s="32" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>18</v>
       </c>
@@ -2846,7 +2864,7 @@
       <c r="AE3" s="29"/>
       <c r="AF3" s="31"/>
     </row>
-    <row r="4" spans="1:32" s="32" customFormat="1">
+    <row r="4" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>18</v>
       </c>
@@ -2894,7 +2912,7 @@
       <c r="AE4" s="29"/>
       <c r="AF4" s="31"/>
     </row>
-    <row r="5" spans="1:32" s="32" customFormat="1">
+    <row r="5" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>32</v>
       </c>
@@ -2944,7 +2962,7 @@
       <c r="AE5" s="29"/>
       <c r="AF5" s="31"/>
     </row>
-    <row r="6" spans="1:32" s="32" customFormat="1">
+    <row r="6" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>32</v>
       </c>
@@ -2992,7 +3010,7 @@
       <c r="AE6" s="29"/>
       <c r="AF6" s="31"/>
     </row>
-    <row r="7" spans="1:32" s="32" customFormat="1">
+    <row r="7" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>11</v>
       </c>
@@ -3042,7 +3060,7 @@
       <c r="AE7" s="29"/>
       <c r="AF7" s="31"/>
     </row>
-    <row r="8" spans="1:32" s="32" customFormat="1">
+    <row r="8" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>11</v>
       </c>
@@ -3092,7 +3110,7 @@
       <c r="AE8" s="29"/>
       <c r="AF8" s="31"/>
     </row>
-    <row r="9" spans="1:32" s="32" customFormat="1">
+    <row r="9" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>7</v>
       </c>
@@ -3142,7 +3160,7 @@
       <c r="AE9" s="29"/>
       <c r="AF9" s="31"/>
     </row>
-    <row r="10" spans="1:32" s="32" customFormat="1">
+    <row r="10" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>7</v>
       </c>
@@ -3192,7 +3210,7 @@
       <c r="AE10" s="29"/>
       <c r="AF10" s="31"/>
     </row>
-    <row r="11" spans="1:32" s="32" customFormat="1">
+    <row r="11" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>6</v>
       </c>
@@ -3242,7 +3260,7 @@
       <c r="AE11" s="29"/>
       <c r="AF11" s="31"/>
     </row>
-    <row r="12" spans="1:32" s="32" customFormat="1">
+    <row r="12" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>6</v>
       </c>
@@ -3288,7 +3306,7 @@
       <c r="AE12" s="29"/>
       <c r="AF12" s="31"/>
     </row>
-    <row r="13" spans="1:32" s="32" customFormat="1">
+    <row r="13" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>34</v>
       </c>
@@ -3338,7 +3356,7 @@
       <c r="AE13" s="29"/>
       <c r="AF13" s="31"/>
     </row>
-    <row r="14" spans="1:32" s="32" customFormat="1">
+    <row r="14" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>34</v>
       </c>
@@ -3386,7 +3404,7 @@
       <c r="AE14" s="29"/>
       <c r="AF14" s="31"/>
     </row>
-    <row r="15" spans="1:32" s="32" customFormat="1">
+    <row r="15" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>38</v>
       </c>
@@ -3436,7 +3454,7 @@
       <c r="AE15" s="29"/>
       <c r="AF15" s="31"/>
     </row>
-    <row r="16" spans="1:32" s="32" customFormat="1">
+    <row r="16" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>38</v>
       </c>
@@ -3486,7 +3504,7 @@
       <c r="AE16" s="29"/>
       <c r="AF16" s="31"/>
     </row>
-    <row r="17" spans="1:33" s="32" customFormat="1">
+    <row r="17" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>89</v>
       </c>
@@ -3536,7 +3554,7 @@
       <c r="AE17" s="29"/>
       <c r="AF17" s="31"/>
     </row>
-    <row r="18" spans="1:33" s="32" customFormat="1">
+    <row r="18" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>89</v>
       </c>
@@ -3586,7 +3604,7 @@
       <c r="AE18" s="29"/>
       <c r="AF18" s="31"/>
     </row>
-    <row r="19" spans="1:33" s="32" customFormat="1">
+    <row r="19" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>184</v>
       </c>
@@ -3637,7 +3655,7 @@
       <c r="AF19" s="51"/>
       <c r="AG19" s="50"/>
     </row>
-    <row r="20" spans="1:33" s="32" customFormat="1">
+    <row r="20" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
         <v>184</v>
       </c>
@@ -3687,7 +3705,7 @@
       <c r="AE20" s="50"/>
       <c r="AF20" s="51"/>
     </row>
-    <row r="21" spans="1:33" s="32" customFormat="1">
+    <row r="21" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
         <v>185</v>
       </c>
@@ -3733,7 +3751,7 @@
       <c r="AE21" s="50"/>
       <c r="AF21" s="51"/>
     </row>
-    <row r="22" spans="1:33" s="32" customFormat="1">
+    <row r="22" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="s">
         <v>185</v>
       </c>
@@ -3783,7 +3801,7 @@
       <c r="AE22" s="50"/>
       <c r="AF22" s="51"/>
     </row>
-    <row r="23" spans="1:33" s="32" customFormat="1">
+    <row r="23" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>193</v>
       </c>
@@ -3833,7 +3851,7 @@
       <c r="AE23" s="50"/>
       <c r="AF23" s="51"/>
     </row>
-    <row r="24" spans="1:33" s="32" customFormat="1">
+    <row r="24" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>193</v>
       </c>
@@ -3881,7 +3899,7 @@
       <c r="AE24" s="50"/>
       <c r="AF24" s="51"/>
     </row>
-    <row r="25" spans="1:33" s="32" customFormat="1">
+    <row r="25" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>202</v>
       </c>
@@ -3931,7 +3949,7 @@
       <c r="AE25" s="50"/>
       <c r="AF25" s="51"/>
     </row>
-    <row r="26" spans="1:33" s="32" customFormat="1">
+    <row r="26" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>202</v>
       </c>
@@ -3979,7 +3997,7 @@
       <c r="AE26" s="50"/>
       <c r="AF26" s="51"/>
     </row>
-    <row r="27" spans="1:33" s="52" customFormat="1">
+    <row r="27" spans="1:33" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>213</v>
       </c>
@@ -4005,7 +4023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:33" s="52" customFormat="1">
+    <row r="28" spans="1:33" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
         <v>213</v>
       </c>
@@ -4025,7 +4043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:33" s="52" customFormat="1">
+    <row r="29" spans="1:33" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="53" t="s">
         <v>222</v>
       </c>
@@ -4051,7 +4069,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:33" s="52" customFormat="1">
+    <row r="30" spans="1:33" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
         <v>222</v>
       </c>
@@ -4071,7 +4089,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:33" s="32" customFormat="1">
+    <row r="31" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
         <v>39</v>
       </c>
@@ -4121,7 +4139,7 @@
       <c r="AE31" s="29"/>
       <c r="AF31" s="31"/>
     </row>
-    <row r="32" spans="1:33" s="32" customFormat="1">
+    <row r="32" spans="1:33" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>39</v>
       </c>
@@ -4171,7 +4189,7 @@
       <c r="AE32" s="29"/>
       <c r="AF32" s="31"/>
     </row>
-    <row r="33" spans="1:32" s="32" customFormat="1">
+    <row r="33" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="53" t="s">
         <v>240</v>
       </c>
@@ -4197,7 +4215,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:32" s="32" customFormat="1">
+    <row r="34" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="53" t="s">
         <v>240</v>
       </c>
@@ -4210,7 +4228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:32" s="32" customFormat="1">
+    <row r="35" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53" t="s">
         <v>42</v>
       </c>
@@ -4260,7 +4278,7 @@
       <c r="AE35" s="29"/>
       <c r="AF35" s="31"/>
     </row>
-    <row r="36" spans="1:32" s="32" customFormat="1">
+    <row r="36" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="66" t="s">
         <v>42</v>
       </c>
@@ -4310,7 +4328,7 @@
       <c r="AE36" s="29"/>
       <c r="AF36" s="31"/>
     </row>
-    <row r="37" spans="1:32" s="32" customFormat="1">
+    <row r="37" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>78</v>
       </c>
@@ -4360,7 +4378,7 @@
       <c r="AE37" s="29"/>
       <c r="AF37" s="31"/>
     </row>
-    <row r="38" spans="1:32" s="32" customFormat="1">
+    <row r="38" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
         <v>78</v>
       </c>
@@ -4410,7 +4428,7 @@
       <c r="AE38" s="29"/>
       <c r="AF38" s="31"/>
     </row>
-    <row r="39" spans="1:32" s="32" customFormat="1">
+    <row r="39" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>12</v>
       </c>
@@ -4458,7 +4476,7 @@
       <c r="AE39" s="29"/>
       <c r="AF39" s="31"/>
     </row>
-    <row r="40" spans="1:32" s="32" customFormat="1">
+    <row r="40" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>12</v>
       </c>
@@ -4506,7 +4524,7 @@
       <c r="AE40" s="29"/>
       <c r="AF40" s="31"/>
     </row>
-    <row r="41" spans="1:32" s="16" customFormat="1">
+    <row r="41" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>36</v>
       </c>
@@ -4554,7 +4572,7 @@
       <c r="AE41" s="13"/>
       <c r="AF41" s="14"/>
     </row>
-    <row r="42" spans="1:32" s="16" customFormat="1">
+    <row r="42" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>36</v>
       </c>
@@ -4602,7 +4620,7 @@
       <c r="AE42" s="13"/>
       <c r="AF42" s="14"/>
     </row>
-    <row r="43" spans="1:32" s="16" customFormat="1">
+    <row r="43" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>36</v>
       </c>
@@ -4650,7 +4668,7 @@
       <c r="AE43" s="13"/>
       <c r="AF43" s="14"/>
     </row>
-    <row r="44" spans="1:32" s="16" customFormat="1">
+    <row r="44" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>36</v>
       </c>
@@ -4698,7 +4716,7 @@
       <c r="AE44" s="13"/>
       <c r="AF44" s="14"/>
     </row>
-    <row r="45" spans="1:32" s="16" customFormat="1">
+    <row r="45" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>53</v>
       </c>
@@ -4746,7 +4764,7 @@
       <c r="AE45" s="13"/>
       <c r="AF45" s="14"/>
     </row>
-    <row r="46" spans="1:32" s="32" customFormat="1">
+    <row r="46" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53" t="s">
         <v>196</v>
       </c>
@@ -4784,7 +4802,7 @@
       <c r="AE46" s="50"/>
       <c r="AF46" s="51"/>
     </row>
-    <row r="47" spans="1:32" s="32" customFormat="1">
+    <row r="47" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="53" t="s">
         <v>196</v>
       </c>
@@ -4822,7 +4840,7 @@
       <c r="AE47" s="50"/>
       <c r="AF47" s="51"/>
     </row>
-    <row r="48" spans="1:32" s="32" customFormat="1">
+    <row r="48" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="53" t="s">
         <v>201</v>
       </c>
@@ -4864,7 +4882,7 @@
       <c r="AE48" s="50"/>
       <c r="AF48" s="51"/>
     </row>
-    <row r="49" spans="1:32" s="32" customFormat="1">
+    <row r="49" spans="1:32" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
         <v>201</v>
       </c>
@@ -4902,7 +4920,7 @@
       <c r="AE49" s="50"/>
       <c r="AF49" s="51"/>
     </row>
-    <row r="50" spans="1:32" s="16" customFormat="1">
+    <row r="50" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>46</v>
       </c>
@@ -4950,7 +4968,7 @@
       <c r="AE50" s="13"/>
       <c r="AF50" s="14"/>
     </row>
-    <row r="51" spans="1:32" s="16" customFormat="1">
+    <row r="51" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>46</v>
       </c>
@@ -4998,7 +5016,7 @@
       <c r="AE51" s="13"/>
       <c r="AF51" s="14"/>
     </row>
-    <row r="52" spans="1:32" s="16" customFormat="1">
+    <row r="52" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>46</v>
       </c>
@@ -5046,7 +5064,7 @@
       <c r="AE52" s="13"/>
       <c r="AF52" s="14"/>
     </row>
-    <row r="53" spans="1:32" s="16" customFormat="1">
+    <row r="53" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>46</v>
       </c>
@@ -5094,7 +5112,7 @@
       <c r="AE53" s="13"/>
       <c r="AF53" s="14"/>
     </row>
-    <row r="54" spans="1:32" s="16" customFormat="1">
+    <row r="54" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>46</v>
       </c>
@@ -5142,7 +5160,7 @@
       <c r="AE54" s="13"/>
       <c r="AF54" s="14"/>
     </row>
-    <row r="55" spans="1:32" s="16" customFormat="1">
+    <row r="55" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>114</v>
       </c>
@@ -5182,7 +5200,7 @@
       <c r="AE55" s="13"/>
       <c r="AF55" s="14"/>
     </row>
-    <row r="56" spans="1:32" s="16" customFormat="1">
+    <row r="56" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>114</v>
       </c>
@@ -5222,7 +5240,7 @@
       <c r="AE56" s="13"/>
       <c r="AF56" s="14"/>
     </row>
-    <row r="57" spans="1:32" s="16" customFormat="1">
+    <row r="57" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>114</v>
       </c>
@@ -5262,7 +5280,7 @@
       <c r="AE57" s="13"/>
       <c r="AF57" s="14"/>
     </row>
-    <row r="58" spans="1:32" s="16" customFormat="1">
+    <row r="58" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>114</v>
       </c>
@@ -5302,7 +5320,7 @@
       <c r="AE58" s="13"/>
       <c r="AF58" s="14"/>
     </row>
-    <row r="59" spans="1:32" s="52" customFormat="1">
+    <row r="59" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="53" t="s">
         <v>212</v>
       </c>
@@ -5342,7 +5360,7 @@
       <c r="AE59" s="59"/>
       <c r="AF59" s="59"/>
     </row>
-    <row r="60" spans="1:32" s="52" customFormat="1">
+    <row r="60" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="53" t="s">
         <v>212</v>
       </c>
@@ -5382,7 +5400,7 @@
       <c r="AE60" s="59"/>
       <c r="AF60" s="59"/>
     </row>
-    <row r="61" spans="1:32" s="52" customFormat="1">
+    <row r="61" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="53" t="s">
         <v>223</v>
       </c>
@@ -5393,7 +5411,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="62" spans="1:32" s="52" customFormat="1">
+    <row r="62" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="53" t="s">
         <v>223</v>
       </c>
@@ -5404,20 +5422,20 @@
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:32" s="52" customFormat="1">
+    <row r="63" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="53" t="s">
         <v>229</v>
       </c>
       <c r="B63" s="53"/>
       <c r="D63" s="61"/>
     </row>
-    <row r="64" spans="1:32" s="52" customFormat="1">
+    <row r="64" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="53" t="s">
         <v>229</v>
       </c>
       <c r="D64" s="61"/>
     </row>
-    <row r="65" spans="1:32" s="52" customFormat="1">
+    <row r="65" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="53" t="s">
         <v>230</v>
       </c>
@@ -5428,7 +5446,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:32" s="52" customFormat="1">
+    <row r="66" spans="1:32" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="53" t="s">
         <v>230</v>
       </c>
@@ -5438,126 +5456,111 @@
       <c r="D66" s="63" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="67" spans="1:32" s="16" customFormat="1">
-      <c r="A67" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C67" s="10"/>
-      <c r="D67" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E67" s="12">
-        <v>1</v>
-      </c>
-      <c r="F67" s="12">
-        <v>400</v>
-      </c>
-      <c r="G67" s="13">
-        <v>48</v>
-      </c>
-      <c r="H67" s="19"/>
-      <c r="I67" s="13">
-        <v>20</v>
-      </c>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="13"/>
-      <c r="S67" s="13"/>
-      <c r="T67" s="13"/>
-      <c r="U67" s="13"/>
-      <c r="V67" s="13"/>
-      <c r="W67" s="13"/>
-      <c r="X67" s="13"/>
-      <c r="Y67" s="13"/>
-      <c r="Z67" s="13"/>
-      <c r="AA67" s="13"/>
-      <c r="AB67" s="13"/>
-      <c r="AC67" s="13"/>
-      <c r="AD67" s="13"/>
-      <c r="AE67" s="13"/>
-      <c r="AF67" s="14"/>
-    </row>
-    <row r="68" spans="1:32" s="16" customFormat="1">
-      <c r="A68" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="10"/>
-      <c r="D68" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E68" s="12">
-        <v>1</v>
-      </c>
-      <c r="F68" s="12">
-        <v>400</v>
-      </c>
-      <c r="G68" s="13">
-        <v>48</v>
-      </c>
-      <c r="H68" s="19"/>
-      <c r="I68" s="13">
-        <v>40</v>
-      </c>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="13"/>
-      <c r="R68" s="13"/>
-      <c r="S68" s="13"/>
-      <c r="T68" s="13"/>
-      <c r="U68" s="13"/>
-      <c r="V68" s="13"/>
-      <c r="W68" s="13"/>
-      <c r="X68" s="13"/>
-      <c r="Y68" s="13"/>
-      <c r="Z68" s="13"/>
-      <c r="AA68" s="13"/>
-      <c r="AB68" s="13"/>
-      <c r="AC68" s="13"/>
-      <c r="AD68" s="13"/>
-      <c r="AE68" s="13"/>
-      <c r="AF68" s="14"/>
-    </row>
-    <row r="69" spans="1:32" s="16" customFormat="1">
+      <c r="AF66" s="62"/>
+    </row>
+    <row r="67" spans="1:32" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" s="62" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="52"/>
+      <c r="D67" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="E67" s="52"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="52"/>
+      <c r="H67" s="52"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
+      <c r="K67" s="52"/>
+      <c r="L67" s="52"/>
+      <c r="M67" s="52"/>
+      <c r="N67" s="52"/>
+      <c r="O67" s="52"/>
+      <c r="P67" s="52"/>
+      <c r="Q67" s="52"/>
+      <c r="R67" s="52"/>
+      <c r="S67" s="52"/>
+      <c r="T67" s="52"/>
+      <c r="U67" s="52"/>
+      <c r="V67" s="52"/>
+      <c r="W67" s="52"/>
+      <c r="X67" s="52"/>
+      <c r="Y67" s="52"/>
+      <c r="Z67" s="52"/>
+      <c r="AA67" s="52"/>
+      <c r="AB67" s="52"/>
+      <c r="AC67" s="52"/>
+      <c r="AD67" s="52"/>
+      <c r="AE67" s="52"/>
+      <c r="AF67" s="62"/>
+    </row>
+    <row r="68" spans="1:32" s="69" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="B68" s="62" t="s">
+        <v>250</v>
+      </c>
+      <c r="C68" s="52"/>
+      <c r="D68" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="E68" s="52"/>
+      <c r="F68" s="52"/>
+      <c r="G68" s="52"/>
+      <c r="H68" s="52"/>
+      <c r="I68" s="52"/>
+      <c r="J68" s="52"/>
+      <c r="K68" s="52"/>
+      <c r="L68" s="52"/>
+      <c r="M68" s="52"/>
+      <c r="N68" s="52"/>
+      <c r="O68" s="52"/>
+      <c r="P68" s="52"/>
+      <c r="Q68" s="52"/>
+      <c r="R68" s="52"/>
+      <c r="S68" s="52"/>
+      <c r="T68" s="52"/>
+      <c r="U68" s="52"/>
+      <c r="V68" s="52"/>
+      <c r="W68" s="52"/>
+      <c r="X68" s="52"/>
+      <c r="Y68" s="52"/>
+      <c r="Z68" s="52"/>
+      <c r="AA68" s="52"/>
+      <c r="AB68" s="52"/>
+      <c r="AC68" s="52"/>
+      <c r="AD68" s="52"/>
+      <c r="AE68" s="52"/>
+      <c r="AF68" s="62"/>
+    </row>
+    <row r="69" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E69" s="17">
-        <v>0</v>
-      </c>
-      <c r="F69" s="18">
-        <v>0</v>
-      </c>
-      <c r="G69" s="15">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="E69" s="12">
+        <v>1</v>
+      </c>
+      <c r="F69" s="12">
+        <v>400</v>
+      </c>
+      <c r="G69" s="13">
+        <v>48</v>
       </c>
       <c r="H69" s="19"/>
-      <c r="I69" s="15">
-        <v>0</v>
+      <c r="I69" s="13">
+        <v>20</v>
       </c>
       <c r="J69" s="13"/>
       <c r="K69" s="13"/>
@@ -5583,22 +5586,30 @@
       <c r="AE69" s="13"/>
       <c r="AF69" s="14"/>
     </row>
-    <row r="70" spans="1:32" s="16" customFormat="1">
+    <row r="70" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E70" s="17"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="15"/>
+        <v>23</v>
+      </c>
+      <c r="E70" s="12">
+        <v>1</v>
+      </c>
+      <c r="F70" s="12">
+        <v>400</v>
+      </c>
+      <c r="G70" s="13">
+        <v>48</v>
+      </c>
       <c r="H70" s="19"/>
-      <c r="I70" s="13"/>
+      <c r="I70" s="13">
+        <v>40</v>
+      </c>
       <c r="J70" s="13"/>
       <c r="K70" s="13"/>
       <c r="L70" s="13"/>
@@ -5623,22 +5634,30 @@
       <c r="AE70" s="13"/>
       <c r="AF70" s="14"/>
     </row>
-    <row r="71" spans="1:32" s="16" customFormat="1">
+    <row r="71" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>144</v>
+        <v>76</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="15"/>
+        <v>77</v>
+      </c>
+      <c r="E71" s="17">
+        <v>0</v>
+      </c>
+      <c r="F71" s="18">
+        <v>0</v>
+      </c>
+      <c r="G71" s="15">
+        <v>0</v>
+      </c>
       <c r="H71" s="19"/>
-      <c r="I71" s="13"/>
+      <c r="I71" s="15">
+        <v>0</v>
+      </c>
       <c r="J71" s="13"/>
       <c r="K71" s="13"/>
       <c r="L71" s="13"/>
@@ -5663,16 +5682,16 @@
       <c r="AE71" s="13"/>
       <c r="AF71" s="14"/>
     </row>
-    <row r="72" spans="1:32" s="16" customFormat="1">
+    <row r="72" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E72" s="17"/>
       <c r="F72" s="18"/>
@@ -5703,16 +5722,16 @@
       <c r="AE72" s="13"/>
       <c r="AF72" s="14"/>
     </row>
-    <row r="73" spans="1:32" s="16" customFormat="1">
+    <row r="73" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="11" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E73" s="17"/>
       <c r="F73" s="18"/>
@@ -5743,16 +5762,16 @@
       <c r="AE73" s="13"/>
       <c r="AF73" s="14"/>
     </row>
-    <row r="74" spans="1:32" s="16" customFormat="1">
+    <row r="74" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="11" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E74" s="17"/>
       <c r="F74" s="18"/>
@@ -5783,30 +5802,22 @@
       <c r="AE74" s="13"/>
       <c r="AF74" s="14"/>
     </row>
-    <row r="75" spans="1:32" s="16" customFormat="1">
+    <row r="75" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E75" s="17">
-        <v>0</v>
-      </c>
-      <c r="F75" s="18">
-        <v>0</v>
-      </c>
-      <c r="G75" s="15">
-        <v>0</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E75" s="17"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="15"/>
       <c r="H75" s="19"/>
-      <c r="I75" s="13">
-        <v>0</v>
-      </c>
+      <c r="I75" s="13"/>
       <c r="J75" s="13"/>
       <c r="K75" s="13"/>
       <c r="L75" s="13"/>
@@ -5831,30 +5842,22 @@
       <c r="AE75" s="13"/>
       <c r="AF75" s="14"/>
     </row>
-    <row r="76" spans="1:32" s="16" customFormat="1">
+    <row r="76" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E76" s="17">
-        <v>0</v>
-      </c>
-      <c r="F76" s="18">
-        <v>0</v>
-      </c>
-      <c r="G76" s="15">
-        <v>0</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E76" s="17"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="15"/>
       <c r="H76" s="19"/>
-      <c r="I76" s="13">
-        <v>0</v>
-      </c>
+      <c r="I76" s="13"/>
       <c r="J76" s="13"/>
       <c r="K76" s="13"/>
       <c r="L76" s="13"/>
@@ -5879,16 +5882,16 @@
       <c r="AE76" s="13"/>
       <c r="AF76" s="14"/>
     </row>
-    <row r="77" spans="1:32" s="16" customFormat="1">
-      <c r="A77" s="54" t="s">
+    <row r="77" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C77" s="10"/>
       <c r="D77" s="11" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E77" s="17">
         <v>0</v>
@@ -5927,63 +5930,73 @@
       <c r="AE77" s="13"/>
       <c r="AF77" s="14"/>
     </row>
-    <row r="78" spans="1:32" s="16" customFormat="1">
-      <c r="A78" s="57"/>
-      <c r="B78" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="C78" s="20"/>
-      <c r="D78" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E78" s="22"/>
-      <c r="F78" s="22"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="23"/>
-      <c r="I78" s="24"/>
-      <c r="J78" s="24"/>
-      <c r="K78" s="24"/>
-      <c r="L78" s="24"/>
-      <c r="M78" s="24"/>
-      <c r="N78" s="24"/>
-      <c r="O78" s="24"/>
-      <c r="P78" s="24"/>
-      <c r="Q78" s="24"/>
-      <c r="R78" s="24"/>
-      <c r="S78" s="24"/>
-      <c r="T78" s="24"/>
-      <c r="U78" s="24"/>
-      <c r="V78" s="24"/>
-      <c r="W78" s="24"/>
-      <c r="X78" s="24"/>
-      <c r="Y78" s="24"/>
-      <c r="Z78" s="24"/>
-      <c r="AA78" s="24"/>
-      <c r="AB78" s="24"/>
-      <c r="AC78" s="24"/>
-      <c r="AD78" s="24"/>
-      <c r="AE78" s="24"/>
-      <c r="AF78" s="25"/>
-    </row>
-    <row r="79" spans="1:32" s="16" customFormat="1">
-      <c r="A79" s="10" t="s">
+    <row r="78" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>25</v>
       </c>
+      <c r="B78" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" s="10"/>
+      <c r="D78" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E78" s="17">
+        <v>0</v>
+      </c>
+      <c r="F78" s="18">
+        <v>0</v>
+      </c>
+      <c r="G78" s="15">
+        <v>0</v>
+      </c>
+      <c r="H78" s="19"/>
+      <c r="I78" s="13">
+        <v>0</v>
+      </c>
+      <c r="J78" s="13"/>
+      <c r="K78" s="13"/>
+      <c r="L78" s="13"/>
+      <c r="M78" s="13"/>
+      <c r="N78" s="13"/>
+      <c r="O78" s="13"/>
+      <c r="P78" s="13"/>
+      <c r="Q78" s="13"/>
+      <c r="R78" s="13"/>
+      <c r="S78" s="13"/>
+      <c r="T78" s="13"/>
+      <c r="U78" s="13"/>
+      <c r="V78" s="13"/>
+      <c r="W78" s="13"/>
+      <c r="X78" s="13"/>
+      <c r="Y78" s="13"/>
+      <c r="Z78" s="13"/>
+      <c r="AA78" s="13"/>
+      <c r="AB78" s="13"/>
+      <c r="AC78" s="13"/>
+      <c r="AD78" s="13"/>
+      <c r="AE78" s="13"/>
+      <c r="AF78" s="14"/>
+    </row>
+    <row r="79" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="54" t="s">
+        <v>25</v>
+      </c>
       <c r="B79" s="10" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="C79" s="10"/>
       <c r="D79" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E79" s="12">
-        <v>1</v>
-      </c>
-      <c r="F79" s="12">
+        <v>136</v>
+      </c>
+      <c r="E79" s="17">
         <v>0</v>
       </c>
-      <c r="G79" s="13">
-        <v>720</v>
+      <c r="F79" s="18">
+        <v>0</v>
+      </c>
+      <c r="G79" s="15">
+        <v>0</v>
       </c>
       <c r="H79" s="19"/>
       <c r="I79" s="13">
@@ -6013,73 +6026,63 @@
       <c r="AE79" s="13"/>
       <c r="AF79" s="14"/>
     </row>
-    <row r="80" spans="1:32" s="16" customFormat="1">
-      <c r="A80" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C80" s="10"/>
-      <c r="D80" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E80" s="17">
-        <v>1</v>
-      </c>
-      <c r="F80" s="18">
-        <v>0</v>
-      </c>
-      <c r="G80" s="15">
-        <v>360</v>
-      </c>
-      <c r="H80" s="19"/>
-      <c r="I80" s="15">
-        <v>0</v>
-      </c>
-      <c r="J80" s="13"/>
-      <c r="K80" s="13"/>
-      <c r="L80" s="13"/>
-      <c r="M80" s="13"/>
-      <c r="N80" s="13"/>
-      <c r="O80" s="13"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="13"/>
-      <c r="R80" s="13"/>
-      <c r="S80" s="13"/>
-      <c r="T80" s="13"/>
-      <c r="U80" s="13"/>
-      <c r="V80" s="13"/>
-      <c r="W80" s="13"/>
-      <c r="X80" s="13"/>
-      <c r="Y80" s="13"/>
-      <c r="Z80" s="13"/>
-      <c r="AA80" s="13"/>
-      <c r="AB80" s="13"/>
-      <c r="AC80" s="13"/>
-      <c r="AD80" s="13"/>
-      <c r="AE80" s="13"/>
-      <c r="AF80" s="14"/>
-    </row>
-    <row r="81" spans="1:32" s="16" customFormat="1">
+    <row r="80" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="57"/>
+      <c r="B80" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C80" s="20"/>
+      <c r="D80" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="24"/>
+      <c r="N80" s="24"/>
+      <c r="O80" s="24"/>
+      <c r="P80" s="24"/>
+      <c r="Q80" s="24"/>
+      <c r="R80" s="24"/>
+      <c r="S80" s="24"/>
+      <c r="T80" s="24"/>
+      <c r="U80" s="24"/>
+      <c r="V80" s="24"/>
+      <c r="W80" s="24"/>
+      <c r="X80" s="24"/>
+      <c r="Y80" s="24"/>
+      <c r="Z80" s="24"/>
+      <c r="AA80" s="24"/>
+      <c r="AB80" s="24"/>
+      <c r="AC80" s="24"/>
+      <c r="AD80" s="24"/>
+      <c r="AE80" s="24"/>
+      <c r="AF80" s="25"/>
+    </row>
+    <row r="81" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C81" s="10"/>
       <c r="D81" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E81" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" s="12">
         <v>0</v>
       </c>
       <c r="G81" s="13">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="H81" s="19"/>
       <c r="I81" s="13">
@@ -6109,28 +6112,28 @@
       <c r="AE81" s="13"/>
       <c r="AF81" s="14"/>
     </row>
-    <row r="82" spans="1:32" s="16" customFormat="1">
+    <row r="82" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="C82" s="10"/>
       <c r="D82" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E82" s="12">
+        <v>84</v>
+      </c>
+      <c r="E82" s="17">
+        <v>1</v>
+      </c>
+      <c r="F82" s="18">
         <v>0</v>
       </c>
-      <c r="F82" s="12">
-        <v>0</v>
-      </c>
-      <c r="G82" s="13">
-        <v>0</v>
+      <c r="G82" s="15">
+        <v>360</v>
       </c>
       <c r="H82" s="19"/>
-      <c r="I82" s="13">
+      <c r="I82" s="15">
         <v>0</v>
       </c>
       <c r="J82" s="13"/>
@@ -6157,16 +6160,16 @@
       <c r="AE82" s="13"/>
       <c r="AF82" s="14"/>
     </row>
-    <row r="83" spans="1:32" s="16" customFormat="1">
+    <row r="83" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E83" s="12">
         <v>0</v>
@@ -6205,16 +6208,16 @@
       <c r="AE83" s="13"/>
       <c r="AF83" s="14"/>
     </row>
-    <row r="84" spans="1:32" s="16" customFormat="1">
+    <row r="84" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E84" s="12">
         <v>0</v>
@@ -6253,6 +6256,102 @@
       <c r="AE84" s="13"/>
       <c r="AF84" s="14"/>
     </row>
+    <row r="85" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="10"/>
+      <c r="D85" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="12">
+        <v>0</v>
+      </c>
+      <c r="F85" s="12">
+        <v>0</v>
+      </c>
+      <c r="G85" s="13">
+        <v>0</v>
+      </c>
+      <c r="H85" s="19"/>
+      <c r="I85" s="13">
+        <v>0</v>
+      </c>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13"/>
+      <c r="O85" s="13"/>
+      <c r="P85" s="13"/>
+      <c r="Q85" s="13"/>
+      <c r="R85" s="13"/>
+      <c r="S85" s="13"/>
+      <c r="T85" s="13"/>
+      <c r="U85" s="13"/>
+      <c r="V85" s="13"/>
+      <c r="W85" s="13"/>
+      <c r="X85" s="13"/>
+      <c r="Y85" s="13"/>
+      <c r="Z85" s="13"/>
+      <c r="AA85" s="13"/>
+      <c r="AB85" s="13"/>
+      <c r="AC85" s="13"/>
+      <c r="AD85" s="13"/>
+      <c r="AE85" s="13"/>
+      <c r="AF85" s="14"/>
+    </row>
+    <row r="86" spans="1:32" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86" s="10"/>
+      <c r="D86" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E86" s="12">
+        <v>0</v>
+      </c>
+      <c r="F86" s="12">
+        <v>0</v>
+      </c>
+      <c r="G86" s="13">
+        <v>0</v>
+      </c>
+      <c r="H86" s="19"/>
+      <c r="I86" s="13">
+        <v>0</v>
+      </c>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+      <c r="N86" s="13"/>
+      <c r="O86" s="13"/>
+      <c r="P86" s="13"/>
+      <c r="Q86" s="13"/>
+      <c r="R86" s="13"/>
+      <c r="S86" s="13"/>
+      <c r="T86" s="13"/>
+      <c r="U86" s="13"/>
+      <c r="V86" s="13"/>
+      <c r="W86" s="13"/>
+      <c r="X86" s="13"/>
+      <c r="Y86" s="13"/>
+      <c r="Z86" s="13"/>
+      <c r="AA86" s="13"/>
+      <c r="AB86" s="13"/>
+      <c r="AC86" s="13"/>
+      <c r="AD86" s="13"/>
+      <c r="AE86" s="13"/>
+      <c r="AF86" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6263,24 +6362,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>